<commit_message>
Súly és méretkorlátozások folyamatban I.
git-tfs-id: [https://gyorgyiantal.visualstudio.com]$/PMap/PMap;C563
</commit_message>
<xml_diff>
--- a/doc/FTLSupporter adatszerkezetek.xlsx
+++ b/doc/FTLSupporter adatszerkezetek.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="358">
   <si>
     <t>Megnevezés</t>
   </si>
@@ -1842,6 +1842,21 @@
   <si>
     <t>DrivingDuration</t>
   </si>
+  <si>
+    <t>Szélesség</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Magasság</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>cm-ben, 0=nincs megadva</t>
+  </si>
 </sst>
 </file>
 
@@ -2002,7 +2017,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2090,6 +2105,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2375,10 +2393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB207"/>
+  <dimension ref="A1:AB209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B147" sqref="B147"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
@@ -3852,22 +3870,22 @@
       <c r="AA45" s="8"/>
       <c r="AB45" s="8"/>
     </row>
-    <row r="46" spans="1:28" ht="25.5">
-      <c r="A46" s="11" t="s">
-        <v>296</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>297</v>
+    <row r="46" spans="1:28">
+      <c r="A46" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>354</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>134</v>
+        <v>26</v>
       </c>
       <c r="D46" s="8" t="s">
         <v>15</v>
       </c>
       <c r="E46" s="8"/>
-      <c r="F46" s="19" t="s">
-        <v>300</v>
+      <c r="F46" s="31" t="s">
+        <v>357</v>
       </c>
       <c r="G46" s="8"/>
       <c r="H46" s="8"/>
@@ -3893,12 +3911,22 @@
       <c r="AB46" s="8"/>
     </row>
     <row r="47" spans="1:28">
-      <c r="A47" s="11"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
+      <c r="A47" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="E47" s="8"/>
-      <c r="F47" s="19"/>
+      <c r="F47" s="31" t="s">
+        <v>357</v>
+      </c>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
       <c r="I47" s="8"/>
@@ -3922,58 +3950,56 @@
       <c r="AA47" s="8"/>
       <c r="AB47" s="8"/>
     </row>
-    <row r="48" spans="1:28">
-      <c r="A48" s="30" t="s">
-        <v>344</v>
-      </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
-      <c r="O48" s="3"/>
-      <c r="P48" s="3"/>
-      <c r="Q48" s="3"/>
-      <c r="R48" s="3"/>
-      <c r="S48" s="3"/>
-      <c r="T48" s="3"/>
-      <c r="U48" s="3"/>
-      <c r="V48" s="3"/>
-      <c r="W48" s="3"/>
-      <c r="X48" s="3"/>
-      <c r="Y48" s="3"/>
-      <c r="Z48" s="3"/>
-      <c r="AA48" s="3"/>
-      <c r="AB48" s="3"/>
-    </row>
-    <row r="49" spans="1:28" ht="51.75" customHeight="1">
-      <c r="A49" s="29" t="s">
-        <v>306</v>
-      </c>
-      <c r="B49" s="29" t="s">
-        <v>305</v>
-      </c>
-      <c r="C49" t="s">
-        <v>26</v>
-      </c>
-      <c r="D49" t="s">
-        <v>12</v>
-      </c>
+    <row r="48" spans="1:28" ht="25.5">
+      <c r="A48" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="8"/>
+      <c r="F48" s="19" t="s">
+        <v>300</v>
+      </c>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="8"/>
+      <c r="M48" s="8"/>
+      <c r="N48" s="8"/>
+      <c r="O48" s="8"/>
+      <c r="P48" s="8"/>
+      <c r="Q48" s="8"/>
+      <c r="R48" s="8"/>
+      <c r="S48" s="8"/>
+      <c r="T48" s="8"/>
+      <c r="U48" s="8"/>
+      <c r="V48" s="8"/>
+      <c r="W48" s="8"/>
+      <c r="X48" s="8"/>
+      <c r="Y48" s="8"/>
+      <c r="Z48" s="8"/>
+      <c r="AA48" s="8"/>
+      <c r="AB48" s="8"/>
+    </row>
+    <row r="49" spans="1:28">
+      <c r="A49" s="11"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
       <c r="E49" s="8"/>
-      <c r="F49" s="31" t="s">
-        <v>343</v>
-      </c>
-      <c r="G49" s="31"/>
-      <c r="H49" s="31"/>
-      <c r="I49" s="31"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
       <c r="J49" s="8"/>
       <c r="K49" s="8"/>
       <c r="L49" s="8"/>
@@ -3995,61 +4021,57 @@
       <c r="AB49" s="8"/>
     </row>
     <row r="50" spans="1:28">
-      <c r="A50" s="29" t="s">
-        <v>317</v>
-      </c>
-      <c r="B50" s="29" t="s">
-        <v>307</v>
-      </c>
-      <c r="C50" t="s">
-        <v>26</v>
-      </c>
-      <c r="D50" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="E50" s="8"/>
-      <c r="F50" s="31"/>
-      <c r="G50" s="31"/>
-      <c r="H50" s="31"/>
-      <c r="I50" s="31"/>
-      <c r="J50" s="8"/>
-      <c r="K50" s="8"/>
-      <c r="L50" s="8"/>
-      <c r="M50" s="8"/>
-      <c r="N50" s="8"/>
-      <c r="O50" s="8"/>
-      <c r="P50" s="8"/>
-      <c r="Q50" s="8"/>
-      <c r="R50" s="8"/>
-      <c r="S50" s="8"/>
-      <c r="T50" s="8"/>
-      <c r="U50" s="8"/>
-      <c r="V50" s="8"/>
-      <c r="W50" s="8"/>
-      <c r="X50" s="8"/>
-      <c r="Y50" s="8"/>
-      <c r="Z50" s="8"/>
-      <c r="AA50" s="8"/>
-      <c r="AB50" s="8"/>
-    </row>
-    <row r="51" spans="1:28">
+      <c r="A50" s="30" t="s">
+        <v>344</v>
+      </c>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="3"/>
+      <c r="O50" s="3"/>
+      <c r="P50" s="3"/>
+      <c r="Q50" s="3"/>
+      <c r="R50" s="3"/>
+      <c r="S50" s="3"/>
+      <c r="T50" s="3"/>
+      <c r="U50" s="3"/>
+      <c r="V50" s="3"/>
+      <c r="W50" s="3"/>
+      <c r="X50" s="3"/>
+      <c r="Y50" s="3"/>
+      <c r="Z50" s="3"/>
+      <c r="AA50" s="3"/>
+      <c r="AB50" s="3"/>
+    </row>
+    <row r="51" spans="1:28" ht="51.75" customHeight="1">
       <c r="A51" s="29" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="B51" s="29" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="C51" t="s">
         <v>26</v>
       </c>
       <c r="D51" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E51" s="8"/>
-      <c r="F51" s="31"/>
-      <c r="G51" s="31"/>
-      <c r="H51" s="31"/>
-      <c r="I51" s="31"/>
+      <c r="F51" s="32" t="s">
+        <v>343</v>
+      </c>
+      <c r="G51" s="32"/>
+      <c r="H51" s="32"/>
+      <c r="I51" s="32"/>
       <c r="J51" s="8"/>
       <c r="K51" s="8"/>
       <c r="L51" s="8"/>
@@ -4070,24 +4092,24 @@
       <c r="AA51" s="8"/>
       <c r="AB51" s="8"/>
     </row>
-    <row r="52" spans="1:28" ht="17.25" customHeight="1">
+    <row r="52" spans="1:28">
       <c r="A52" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="B52" t="s">
-        <v>308</v>
+        <v>317</v>
+      </c>
+      <c r="B52" s="29" t="s">
+        <v>307</v>
       </c>
       <c r="C52" t="s">
         <v>26</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="29" t="s">
         <v>15</v>
       </c>
       <c r="E52" s="8"/>
-      <c r="F52" s="31"/>
-      <c r="G52" s="31"/>
-      <c r="H52" s="31"/>
-      <c r="I52" s="31"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="32"/>
+      <c r="I52" s="32"/>
       <c r="J52" s="8"/>
       <c r="K52" s="8"/>
       <c r="L52" s="8"/>
@@ -4108,12 +4130,12 @@
       <c r="AA52" s="8"/>
       <c r="AB52" s="8"/>
     </row>
-    <row r="53" spans="1:28" ht="15.75" customHeight="1">
+    <row r="53" spans="1:28">
       <c r="A53" s="29" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B53" s="29" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="C53" t="s">
         <v>26</v>
@@ -4122,10 +4144,10 @@
         <v>15</v>
       </c>
       <c r="E53" s="8"/>
-      <c r="F53" s="31"/>
-      <c r="G53" s="31"/>
-      <c r="H53" s="31"/>
-      <c r="I53" s="31"/>
+      <c r="F53" s="32"/>
+      <c r="G53" s="32"/>
+      <c r="H53" s="32"/>
+      <c r="I53" s="32"/>
       <c r="J53" s="8"/>
       <c r="K53" s="8"/>
       <c r="L53" s="8"/>
@@ -4146,12 +4168,12 @@
       <c r="AA53" s="8"/>
       <c r="AB53" s="8"/>
     </row>
-    <row r="54" spans="1:28">
+    <row r="54" spans="1:28" ht="17.25" customHeight="1">
       <c r="A54" s="29" t="s">
-        <v>330</v>
-      </c>
-      <c r="B54" s="29" t="s">
-        <v>311</v>
+        <v>309</v>
+      </c>
+      <c r="B54" t="s">
+        <v>308</v>
       </c>
       <c r="C54" t="s">
         <v>26</v>
@@ -4160,10 +4182,10 @@
         <v>15</v>
       </c>
       <c r="E54" s="8"/>
-      <c r="F54" s="31"/>
-      <c r="G54" s="31"/>
-      <c r="H54" s="31"/>
-      <c r="I54" s="31"/>
+      <c r="F54" s="32"/>
+      <c r="G54" s="32"/>
+      <c r="H54" s="32"/>
+      <c r="I54" s="32"/>
       <c r="J54" s="8"/>
       <c r="K54" s="8"/>
       <c r="L54" s="8"/>
@@ -4184,12 +4206,12 @@
       <c r="AA54" s="8"/>
       <c r="AB54" s="8"/>
     </row>
-    <row r="55" spans="1:28">
+    <row r="55" spans="1:28" ht="15.75" customHeight="1">
       <c r="A55" s="29" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="B55" s="29" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C55" t="s">
         <v>26</v>
@@ -4198,10 +4220,10 @@
         <v>15</v>
       </c>
       <c r="E55" s="8"/>
-      <c r="F55" s="31"/>
-      <c r="G55" s="31"/>
-      <c r="H55" s="31"/>
-      <c r="I55" s="31"/>
+      <c r="F55" s="32"/>
+      <c r="G55" s="32"/>
+      <c r="H55" s="32"/>
+      <c r="I55" s="32"/>
       <c r="J55" s="8"/>
       <c r="K55" s="8"/>
       <c r="L55" s="8"/>
@@ -4224,10 +4246,10 @@
     </row>
     <row r="56" spans="1:28">
       <c r="A56" s="29" t="s">
-        <v>318</v>
+        <v>330</v>
       </c>
       <c r="B56" s="29" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="C56" t="s">
         <v>26</v>
@@ -4236,10 +4258,10 @@
         <v>15</v>
       </c>
       <c r="E56" s="8"/>
-      <c r="F56" s="31"/>
-      <c r="G56" s="31"/>
-      <c r="H56" s="31"/>
-      <c r="I56" s="31"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="32"/>
+      <c r="I56" s="32"/>
       <c r="J56" s="8"/>
       <c r="K56" s="8"/>
       <c r="L56" s="8"/>
@@ -4262,10 +4284,10 @@
     </row>
     <row r="57" spans="1:28">
       <c r="A57" s="29" t="s">
-        <v>319</v>
+        <v>329</v>
       </c>
       <c r="B57" s="29" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="C57" t="s">
         <v>26</v>
@@ -4274,10 +4296,10 @@
         <v>15</v>
       </c>
       <c r="E57" s="8"/>
-      <c r="F57" s="31"/>
-      <c r="G57" s="31"/>
-      <c r="H57" s="31"/>
-      <c r="I57" s="31"/>
+      <c r="F57" s="32"/>
+      <c r="G57" s="32"/>
+      <c r="H57" s="32"/>
+      <c r="I57" s="32"/>
       <c r="J57" s="8"/>
       <c r="K57" s="8"/>
       <c r="L57" s="8"/>
@@ -4298,12 +4320,12 @@
       <c r="AA57" s="8"/>
       <c r="AB57" s="8"/>
     </row>
-    <row r="58" spans="1:28" ht="38.25">
-      <c r="A58" s="28" t="s">
-        <v>322</v>
-      </c>
-      <c r="B58" t="s">
-        <v>313</v>
+    <row r="58" spans="1:28">
+      <c r="A58" s="29" t="s">
+        <v>318</v>
+      </c>
+      <c r="B58" s="29" t="s">
+        <v>320</v>
       </c>
       <c r="C58" t="s">
         <v>26</v>
@@ -4312,10 +4334,10 @@
         <v>15</v>
       </c>
       <c r="E58" s="8"/>
-      <c r="F58" s="31"/>
-      <c r="G58" s="31"/>
-      <c r="H58" s="31"/>
-      <c r="I58" s="31"/>
+      <c r="F58" s="32"/>
+      <c r="G58" s="32"/>
+      <c r="H58" s="32"/>
+      <c r="I58" s="32"/>
       <c r="J58" s="8"/>
       <c r="K58" s="8"/>
       <c r="L58" s="8"/>
@@ -4337,15 +4359,23 @@
       <c r="AB58" s="8"/>
     </row>
     <row r="59" spans="1:28">
-      <c r="A59" s="29"/>
-      <c r="B59" s="29"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="11"/>
+      <c r="A59" s="29" t="s">
+        <v>319</v>
+      </c>
+      <c r="B59" s="29" t="s">
+        <v>321</v>
+      </c>
+      <c r="C59" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" t="s">
+        <v>15</v>
+      </c>
       <c r="E59" s="8"/>
-      <c r="F59" s="19"/>
-      <c r="G59" s="19"/>
-      <c r="H59" s="19"/>
-      <c r="I59" s="19"/>
+      <c r="F59" s="32"/>
+      <c r="G59" s="32"/>
+      <c r="H59" s="32"/>
+      <c r="I59" s="32"/>
       <c r="J59" s="8"/>
       <c r="K59" s="8"/>
       <c r="L59" s="8"/>
@@ -4366,58 +4396,54 @@
       <c r="AA59" s="8"/>
       <c r="AB59" s="8"/>
     </row>
-    <row r="60" spans="1:28">
-      <c r="A60" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="17"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
-      <c r="I60" s="3"/>
-      <c r="J60" s="3"/>
-      <c r="K60" s="3"/>
-      <c r="L60" s="3"/>
-      <c r="M60" s="3"/>
-      <c r="N60" s="3"/>
-      <c r="O60" s="3"/>
-      <c r="P60" s="3"/>
-      <c r="Q60" s="3"/>
-      <c r="R60" s="3"/>
-      <c r="S60" s="3"/>
-      <c r="T60" s="3"/>
-      <c r="U60" s="3"/>
-      <c r="V60" s="3"/>
-      <c r="W60" s="3"/>
-      <c r="X60" s="3"/>
-      <c r="Y60" s="3"/>
-      <c r="Z60" s="3"/>
-      <c r="AA60" s="3"/>
-      <c r="AB60" s="3"/>
-    </row>
-    <row r="61" spans="1:28" ht="178.5">
-      <c r="A61" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>12</v>
-      </c>
+    <row r="60" spans="1:28" ht="38.25">
+      <c r="A60" s="28" t="s">
+        <v>322</v>
+      </c>
+      <c r="B60" t="s">
+        <v>313</v>
+      </c>
+      <c r="C60" t="s">
+        <v>26</v>
+      </c>
+      <c r="D60" t="s">
+        <v>15</v>
+      </c>
+      <c r="E60" s="8"/>
+      <c r="F60" s="32"/>
+      <c r="G60" s="32"/>
+      <c r="H60" s="32"/>
+      <c r="I60" s="32"/>
+      <c r="J60" s="8"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="8"/>
+      <c r="M60" s="8"/>
+      <c r="N60" s="8"/>
+      <c r="O60" s="8"/>
+      <c r="P60" s="8"/>
+      <c r="Q60" s="8"/>
+      <c r="R60" s="8"/>
+      <c r="S60" s="8"/>
+      <c r="T60" s="8"/>
+      <c r="U60" s="8"/>
+      <c r="V60" s="8"/>
+      <c r="W60" s="8"/>
+      <c r="X60" s="8"/>
+      <c r="Y60" s="8"/>
+      <c r="Z60" s="8"/>
+      <c r="AA60" s="8"/>
+      <c r="AB60" s="8"/>
+    </row>
+    <row r="61" spans="1:28">
+      <c r="A61" s="29"/>
+      <c r="B61" s="29"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="11"/>
       <c r="E61" s="8"/>
-      <c r="F61" s="19" t="s">
-        <v>279</v>
-      </c>
-      <c r="G61" s="8"/>
-      <c r="H61" s="8"/>
-      <c r="I61" s="8"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="19"/>
+      <c r="I61" s="19"/>
       <c r="J61" s="8"/>
       <c r="K61" s="8"/>
       <c r="L61" s="8"/>
@@ -4439,61 +4465,53 @@
       <c r="AB61" s="8"/>
     </row>
     <row r="62" spans="1:28">
-      <c r="A62" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D62" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="E62" s="8"/>
-      <c r="F62" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="G62" s="8"/>
-      <c r="H62" s="8"/>
-      <c r="I62" s="8"/>
-      <c r="J62" s="8"/>
-      <c r="K62" s="8"/>
-      <c r="L62" s="8"/>
-      <c r="M62" s="8"/>
-      <c r="N62" s="8"/>
-      <c r="O62" s="8"/>
-      <c r="P62" s="8"/>
-      <c r="Q62" s="8"/>
-      <c r="R62" s="8"/>
-      <c r="S62" s="8"/>
-      <c r="T62" s="8"/>
-      <c r="U62" s="8"/>
-      <c r="V62" s="8"/>
-      <c r="W62" s="8"/>
-      <c r="X62" s="8"/>
-      <c r="Y62" s="8"/>
-      <c r="Z62" s="8"/>
-      <c r="AA62" s="8"/>
-      <c r="AB62" s="8"/>
-    </row>
-    <row r="63" spans="1:28">
-      <c r="A63" s="9" t="s">
-        <v>104</v>
+      <c r="A62" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="3"/>
+      <c r="N62" s="3"/>
+      <c r="O62" s="3"/>
+      <c r="P62" s="3"/>
+      <c r="Q62" s="3"/>
+      <c r="R62" s="3"/>
+      <c r="S62" s="3"/>
+      <c r="T62" s="3"/>
+      <c r="U62" s="3"/>
+      <c r="V62" s="3"/>
+      <c r="W62" s="3"/>
+      <c r="X62" s="3"/>
+      <c r="Y62" s="3"/>
+      <c r="Z62" s="3"/>
+      <c r="AA62" s="3"/>
+      <c r="AB62" s="3"/>
+    </row>
+    <row r="63" spans="1:28" ht="178.5">
+      <c r="A63" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>102</v>
+        <v>12</v>
       </c>
       <c r="E63" s="8"/>
-      <c r="F63" s="14" t="s">
-        <v>107</v>
+      <c r="F63" s="19" t="s">
+        <v>279</v>
       </c>
       <c r="G63" s="8"/>
       <c r="H63" s="8"/>
@@ -4518,22 +4536,22 @@
       <c r="AA63" s="8"/>
       <c r="AB63" s="8"/>
     </row>
-    <row r="64" spans="1:28" ht="25.5">
+    <row r="64" spans="1:28">
       <c r="A64" s="8" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>110</v>
+        <v>11</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>102</v>
       </c>
       <c r="E64" s="8"/>
-      <c r="F64" s="19" t="s">
-        <v>280</v>
+      <c r="F64" s="14" t="s">
+        <v>103</v>
       </c>
       <c r="G64" s="8"/>
       <c r="H64" s="8"/>
@@ -4558,22 +4576,22 @@
       <c r="AA64" s="8"/>
       <c r="AB64" s="8"/>
     </row>
-    <row r="65" spans="1:28" ht="25.5">
-      <c r="A65" s="8" t="s">
-        <v>111</v>
+    <row r="65" spans="1:28">
+      <c r="A65" s="9" t="s">
+        <v>104</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D65" s="7" t="s">
-        <v>110</v>
+        <v>106</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>102</v>
       </c>
       <c r="E65" s="8"/>
-      <c r="F65" s="20" t="s">
-        <v>113</v>
+      <c r="F65" s="14" t="s">
+        <v>107</v>
       </c>
       <c r="G65" s="8"/>
       <c r="H65" s="8"/>
@@ -4600,20 +4618,20 @@
     </row>
     <row r="66" spans="1:28" ht="25.5">
       <c r="A66" s="8" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D66" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D66" s="9" t="s">
         <v>110</v>
       </c>
       <c r="E66" s="8"/>
-      <c r="F66" s="20" t="s">
-        <v>116</v>
+      <c r="F66" s="19" t="s">
+        <v>280</v>
       </c>
       <c r="G66" s="8"/>
       <c r="H66" s="8"/>
@@ -4638,22 +4656,22 @@
       <c r="AA66" s="8"/>
       <c r="AB66" s="8"/>
     </row>
-    <row r="67" spans="1:28" ht="38.25">
+    <row r="67" spans="1:28" ht="25.5">
       <c r="A67" s="8" t="s">
-        <v>62</v>
+        <v>111</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D67" s="8" t="s">
-        <v>12</v>
+        <v>112</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>110</v>
       </c>
       <c r="E67" s="8"/>
-      <c r="F67" s="14" t="s">
-        <v>118</v>
+      <c r="F67" s="20" t="s">
+        <v>113</v>
       </c>
       <c r="G67" s="8"/>
       <c r="H67" s="8"/>
@@ -4678,208 +4696,216 @@
       <c r="AA67" s="8"/>
       <c r="AB67" s="8"/>
     </row>
-    <row r="68" spans="1:28">
-      <c r="A68" s="10" t="s">
+    <row r="68" spans="1:28" ht="25.5">
+      <c r="A68" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E68" s="8"/>
+      <c r="F68" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
+      <c r="I68" s="8"/>
+      <c r="J68" s="8"/>
+      <c r="K68" s="8"/>
+      <c r="L68" s="8"/>
+      <c r="M68" s="8"/>
+      <c r="N68" s="8"/>
+      <c r="O68" s="8"/>
+      <c r="P68" s="8"/>
+      <c r="Q68" s="8"/>
+      <c r="R68" s="8"/>
+      <c r="S68" s="8"/>
+      <c r="T68" s="8"/>
+      <c r="U68" s="8"/>
+      <c r="V68" s="8"/>
+      <c r="W68" s="8"/>
+      <c r="X68" s="8"/>
+      <c r="Y68" s="8"/>
+      <c r="Z68" s="8"/>
+      <c r="AA68" s="8"/>
+      <c r="AB68" s="8"/>
+    </row>
+    <row r="69" spans="1:28" ht="38.25">
+      <c r="A69" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E69" s="8"/>
+      <c r="F69" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="G69" s="8"/>
+      <c r="H69" s="8"/>
+      <c r="I69" s="8"/>
+      <c r="J69" s="8"/>
+      <c r="K69" s="8"/>
+      <c r="L69" s="8"/>
+      <c r="M69" s="8"/>
+      <c r="N69" s="8"/>
+      <c r="O69" s="8"/>
+      <c r="P69" s="8"/>
+      <c r="Q69" s="8"/>
+      <c r="R69" s="8"/>
+      <c r="S69" s="8"/>
+      <c r="T69" s="8"/>
+      <c r="U69" s="8"/>
+      <c r="V69" s="8"/>
+      <c r="W69" s="8"/>
+      <c r="X69" s="8"/>
+      <c r="Y69" s="8"/>
+      <c r="Z69" s="8"/>
+      <c r="AA69" s="8"/>
+      <c r="AB69" s="8"/>
+    </row>
+    <row r="70" spans="1:28">
+      <c r="A70" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B70" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C68" s="10" t="s">
+      <c r="C70" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D68" s="10" t="s">
+      <c r="D70" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F68" s="15" t="s">
+      <c r="F70" s="15" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="69" spans="1:28">
-      <c r="F69" s="23"/>
-    </row>
-    <row r="70" spans="1:28">
-      <c r="A70" s="8"/>
-      <c r="B70" s="8"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="8"/>
-      <c r="E70" s="8"/>
-      <c r="F70" s="14"/>
-      <c r="G70" s="8"/>
-      <c r="H70" s="8"/>
-      <c r="I70" s="8"/>
-      <c r="J70" s="8"/>
-      <c r="K70" s="8"/>
-      <c r="L70" s="8"/>
-      <c r="M70" s="8"/>
-      <c r="N70" s="8"/>
-      <c r="O70" s="8"/>
-      <c r="P70" s="8"/>
-      <c r="Q70" s="8"/>
-      <c r="R70" s="8"/>
-      <c r="S70" s="8"/>
-      <c r="T70" s="8"/>
-      <c r="U70" s="8"/>
-      <c r="V70" s="8"/>
-      <c r="W70" s="8"/>
-      <c r="X70" s="8"/>
-      <c r="Y70" s="8"/>
-      <c r="Z70" s="8"/>
-      <c r="AA70" s="8"/>
-      <c r="AB70" s="8"/>
-    </row>
     <row r="71" spans="1:28">
-      <c r="A71" s="3" t="s">
+      <c r="F71" s="23"/>
+    </row>
+    <row r="72" spans="1:28">
+      <c r="A72" s="8"/>
+      <c r="B72" s="8"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8"/>
+      <c r="I72" s="8"/>
+      <c r="J72" s="8"/>
+      <c r="K72" s="8"/>
+      <c r="L72" s="8"/>
+      <c r="M72" s="8"/>
+      <c r="N72" s="8"/>
+      <c r="O72" s="8"/>
+      <c r="P72" s="8"/>
+      <c r="Q72" s="8"/>
+      <c r="R72" s="8"/>
+      <c r="S72" s="8"/>
+      <c r="T72" s="8"/>
+      <c r="U72" s="8"/>
+      <c r="V72" s="8"/>
+      <c r="W72" s="8"/>
+      <c r="X72" s="8"/>
+      <c r="Y72" s="8"/>
+      <c r="Z72" s="8"/>
+      <c r="AA72" s="8"/>
+      <c r="AB72" s="8"/>
+    </row>
+    <row r="73" spans="1:28">
+      <c r="A73" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B73" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="17"/>
-      <c r="G71" s="3"/>
-      <c r="H71" s="3"/>
-      <c r="I71" s="3"/>
-      <c r="J71" s="3"/>
-      <c r="K71" s="3"/>
-      <c r="L71" s="3"/>
-      <c r="M71" s="3"/>
-      <c r="N71" s="3"/>
-      <c r="O71" s="3"/>
-      <c r="P71" s="3"/>
-      <c r="Q71" s="3"/>
-      <c r="R71" s="3"/>
-      <c r="S71" s="3"/>
-      <c r="T71" s="3"/>
-      <c r="U71" s="3"/>
-      <c r="V71" s="3"/>
-      <c r="W71" s="3"/>
-      <c r="X71" s="3"/>
-      <c r="Y71" s="3"/>
-      <c r="Z71" s="3"/>
-      <c r="AA71" s="3"/>
-      <c r="AB71" s="3"/>
-    </row>
-    <row r="72" spans="1:28">
-      <c r="A72" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="B72" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="F72" s="23"/>
-    </row>
-    <row r="73" spans="1:28" ht="25.5">
-      <c r="A73" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="B73" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="F73" s="23"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="17"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
+      <c r="M73" s="3"/>
+      <c r="N73" s="3"/>
+      <c r="O73" s="3"/>
+      <c r="P73" s="3"/>
+      <c r="Q73" s="3"/>
+      <c r="R73" s="3"/>
+      <c r="S73" s="3"/>
+      <c r="T73" s="3"/>
+      <c r="U73" s="3"/>
+      <c r="V73" s="3"/>
+      <c r="W73" s="3"/>
+      <c r="X73" s="3"/>
+      <c r="Y73" s="3"/>
+      <c r="Z73" s="3"/>
+      <c r="AA73" s="3"/>
+      <c r="AB73" s="3"/>
     </row>
     <row r="74" spans="1:28">
       <c r="A74" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F74" s="23"/>
+    </row>
+    <row r="75" spans="1:28" ht="25.5">
+      <c r="A75" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="F75" s="23"/>
+    </row>
+    <row r="76" spans="1:28">
+      <c r="A76" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="B74" s="10" t="s">
+      <c r="B76" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="F74" s="23"/>
-    </row>
-    <row r="75" spans="1:28">
-      <c r="A75" s="10" t="s">
+      <c r="F76" s="23"/>
+    </row>
+    <row r="77" spans="1:28">
+      <c r="A77" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="B75" s="10" t="s">
+      <c r="B77" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="F75" s="23"/>
-    </row>
-    <row r="76" spans="1:28">
-      <c r="F76" s="23"/>
-    </row>
-    <row r="77" spans="1:28">
-      <c r="A77" s="8"/>
-      <c r="B77" s="8"/>
-      <c r="C77" s="8"/>
-      <c r="D77" s="9"/>
-      <c r="E77" s="8"/>
-      <c r="F77" s="14"/>
-      <c r="G77" s="8"/>
-      <c r="H77" s="8"/>
-      <c r="I77" s="8"/>
-      <c r="J77" s="8"/>
-      <c r="K77" s="8"/>
-      <c r="L77" s="8"/>
-      <c r="M77" s="8"/>
-      <c r="N77" s="8"/>
-      <c r="O77" s="8"/>
-      <c r="P77" s="8"/>
-      <c r="Q77" s="8"/>
-      <c r="R77" s="8"/>
-      <c r="S77" s="8"/>
-      <c r="T77" s="8"/>
-      <c r="U77" s="8"/>
-      <c r="V77" s="8"/>
-      <c r="W77" s="8"/>
-      <c r="X77" s="8"/>
-      <c r="Y77" s="8"/>
-      <c r="Z77" s="8"/>
-      <c r="AA77" s="8"/>
-      <c r="AB77" s="8"/>
+      <c r="F77" s="23"/>
     </row>
     <row r="78" spans="1:28">
-      <c r="A78" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
-      <c r="E78" s="2"/>
-      <c r="F78" s="13"/>
-      <c r="G78" s="2"/>
-      <c r="H78" s="2"/>
-      <c r="I78" s="2"/>
-      <c r="J78" s="2"/>
-      <c r="K78" s="2"/>
-      <c r="L78" s="2"/>
-      <c r="M78" s="2"/>
-      <c r="N78" s="2"/>
-      <c r="O78" s="2"/>
-      <c r="P78" s="2"/>
-      <c r="Q78" s="2"/>
-      <c r="R78" s="2"/>
-      <c r="S78" s="2"/>
-      <c r="T78" s="2"/>
-      <c r="U78" s="2"/>
-      <c r="V78" s="2"/>
-      <c r="W78" s="2"/>
-      <c r="X78" s="2"/>
-      <c r="Y78" s="2"/>
-      <c r="Z78" s="2"/>
-      <c r="AA78" s="2"/>
-      <c r="AB78" s="2"/>
+      <c r="F78" s="23"/>
     </row>
     <row r="79" spans="1:28">
-      <c r="A79" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B79" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="C79" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D79" s="8"/>
+      <c r="A79" s="8"/>
+      <c r="B79" s="8"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="9"/>
       <c r="E79" s="8"/>
-      <c r="F79" s="14" t="s">
-        <v>135</v>
-      </c>
+      <c r="F79" s="14"/>
       <c r="G79" s="8"/>
       <c r="H79" s="8"/>
       <c r="I79" s="8"/>
@@ -4904,57 +4930,53 @@
       <c r="AB79" s="8"/>
     </row>
     <row r="80" spans="1:28">
-      <c r="A80" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="B80" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D80" s="8"/>
-      <c r="E80" s="8"/>
-      <c r="F80" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="G80" s="8"/>
-      <c r="H80" s="8"/>
-      <c r="I80" s="8"/>
-      <c r="J80" s="8"/>
-      <c r="K80" s="8"/>
-      <c r="L80" s="8"/>
-      <c r="M80" s="8"/>
-      <c r="N80" s="8"/>
-      <c r="O80" s="8"/>
-      <c r="P80" s="8"/>
-      <c r="Q80" s="8"/>
-      <c r="R80" s="8"/>
-      <c r="S80" s="8"/>
-      <c r="T80" s="8"/>
-      <c r="U80" s="8"/>
-      <c r="V80" s="8"/>
-      <c r="W80" s="8"/>
-      <c r="X80" s="8"/>
-      <c r="Y80" s="8"/>
-      <c r="Z80" s="8"/>
-      <c r="AA80" s="8"/>
-      <c r="AB80" s="8"/>
+      <c r="A80" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="13"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
+      <c r="J80" s="2"/>
+      <c r="K80" s="2"/>
+      <c r="L80" s="2"/>
+      <c r="M80" s="2"/>
+      <c r="N80" s="2"/>
+      <c r="O80" s="2"/>
+      <c r="P80" s="2"/>
+      <c r="Q80" s="2"/>
+      <c r="R80" s="2"/>
+      <c r="S80" s="2"/>
+      <c r="T80" s="2"/>
+      <c r="U80" s="2"/>
+      <c r="V80" s="2"/>
+      <c r="W80" s="2"/>
+      <c r="X80" s="2"/>
+      <c r="Y80" s="2"/>
+      <c r="Z80" s="2"/>
+      <c r="AA80" s="2"/>
+      <c r="AB80" s="2"/>
     </row>
     <row r="81" spans="1:28">
       <c r="A81" s="8" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C81" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="D81" s="9"/>
+      <c r="D81" s="8"/>
       <c r="E81" s="8"/>
       <c r="F81" s="14" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="G81" s="8"/>
       <c r="H81" s="8"/>
@@ -4980,12 +5002,20 @@
       <c r="AB81" s="8"/>
     </row>
     <row r="82" spans="1:28">
-      <c r="A82" s="8"/>
-      <c r="B82" s="8"/>
-      <c r="C82" s="8"/>
-      <c r="D82" s="9"/>
+      <c r="A82" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D82" s="8"/>
       <c r="E82" s="8"/>
-      <c r="F82" s="14"/>
+      <c r="F82" s="14" t="s">
+        <v>138</v>
+      </c>
       <c r="G82" s="8"/>
       <c r="H82" s="8"/>
       <c r="I82" s="8"/>
@@ -5010,12 +5040,20 @@
       <c r="AB82" s="8"/>
     </row>
     <row r="83" spans="1:28">
-      <c r="A83" s="8"/>
-      <c r="B83" s="8"/>
-      <c r="C83" s="8"/>
+      <c r="A83" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>134</v>
+      </c>
       <c r="D83" s="9"/>
       <c r="E83" s="8"/>
-      <c r="F83" s="14"/>
+      <c r="F83" s="14" t="s">
+        <v>140</v>
+      </c>
       <c r="G83" s="8"/>
       <c r="H83" s="8"/>
       <c r="I83" s="8"/>
@@ -5040,54 +5078,42 @@
       <c r="AB83" s="8"/>
     </row>
     <row r="84" spans="1:28">
-      <c r="A84" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
-      <c r="F84" s="13"/>
-      <c r="G84" s="2"/>
-      <c r="H84" s="2"/>
-      <c r="I84" s="2"/>
-      <c r="J84" s="2"/>
-      <c r="K84" s="2"/>
-      <c r="L84" s="2"/>
-      <c r="M84" s="2"/>
-      <c r="N84" s="2"/>
-      <c r="O84" s="2"/>
-      <c r="P84" s="2"/>
-      <c r="Q84" s="2"/>
-      <c r="R84" s="2"/>
-      <c r="S84" s="2"/>
-      <c r="T84" s="2"/>
-      <c r="U84" s="2"/>
-      <c r="V84" s="2"/>
-      <c r="W84" s="2"/>
-      <c r="X84" s="2"/>
-      <c r="Y84" s="2"/>
-      <c r="Z84" s="2"/>
-      <c r="AA84" s="2"/>
-      <c r="AB84" s="2"/>
+      <c r="A84" s="8"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="8"/>
+      <c r="F84" s="14"/>
+      <c r="G84" s="8"/>
+      <c r="H84" s="8"/>
+      <c r="I84" s="8"/>
+      <c r="J84" s="8"/>
+      <c r="K84" s="8"/>
+      <c r="L84" s="8"/>
+      <c r="M84" s="8"/>
+      <c r="N84" s="8"/>
+      <c r="O84" s="8"/>
+      <c r="P84" s="8"/>
+      <c r="Q84" s="8"/>
+      <c r="R84" s="8"/>
+      <c r="S84" s="8"/>
+      <c r="T84" s="8"/>
+      <c r="U84" s="8"/>
+      <c r="V84" s="8"/>
+      <c r="W84" s="8"/>
+      <c r="X84" s="8"/>
+      <c r="Y84" s="8"/>
+      <c r="Z84" s="8"/>
+      <c r="AA84" s="8"/>
+      <c r="AB84" s="8"/>
     </row>
     <row r="85" spans="1:28">
-      <c r="A85" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>47</v>
-      </c>
+      <c r="A85" s="8"/>
+      <c r="B85" s="8"/>
+      <c r="C85" s="8"/>
       <c r="D85" s="9"/>
       <c r="E85" s="8"/>
-      <c r="F85" s="14" t="s">
-        <v>144</v>
-      </c>
+      <c r="F85" s="14"/>
       <c r="G85" s="8"/>
       <c r="H85" s="8"/>
       <c r="I85" s="8"/>
@@ -5111,49 +5137,55 @@
       <c r="AA85" s="8"/>
       <c r="AB85" s="8"/>
     </row>
-    <row r="86" spans="1:28" ht="25.5">
-      <c r="A86" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="B86" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="D86" s="9"/>
-      <c r="E86" s="8"/>
-      <c r="F86" s="14"/>
-      <c r="G86" s="8"/>
-      <c r="H86" s="8"/>
-      <c r="I86" s="8"/>
-      <c r="J86" s="8"/>
-      <c r="K86" s="8"/>
-      <c r="L86" s="8"/>
-      <c r="M86" s="8"/>
-      <c r="N86" s="8"/>
-      <c r="O86" s="8"/>
-      <c r="P86" s="8"/>
-      <c r="Q86" s="8"/>
-      <c r="R86" s="8"/>
-      <c r="S86" s="8"/>
-      <c r="T86" s="8"/>
-      <c r="U86" s="8"/>
-      <c r="V86" s="8"/>
-      <c r="W86" s="8"/>
-      <c r="X86" s="8"/>
-      <c r="Y86" s="8"/>
-      <c r="Z86" s="8"/>
-      <c r="AA86" s="8"/>
-      <c r="AB86" s="8"/>
+    <row r="86" spans="1:28">
+      <c r="A86" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="13"/>
+      <c r="G86" s="2"/>
+      <c r="H86" s="2"/>
+      <c r="I86" s="2"/>
+      <c r="J86" s="2"/>
+      <c r="K86" s="2"/>
+      <c r="L86" s="2"/>
+      <c r="M86" s="2"/>
+      <c r="N86" s="2"/>
+      <c r="O86" s="2"/>
+      <c r="P86" s="2"/>
+      <c r="Q86" s="2"/>
+      <c r="R86" s="2"/>
+      <c r="S86" s="2"/>
+      <c r="T86" s="2"/>
+      <c r="U86" s="2"/>
+      <c r="V86" s="2"/>
+      <c r="W86" s="2"/>
+      <c r="X86" s="2"/>
+      <c r="Y86" s="2"/>
+      <c r="Z86" s="2"/>
+      <c r="AA86" s="2"/>
+      <c r="AB86" s="2"/>
     </row>
     <row r="87" spans="1:28">
-      <c r="A87" s="8"/>
-      <c r="B87" s="8"/>
-      <c r="C87" s="8"/>
+      <c r="A87" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="D87" s="9"/>
       <c r="E87" s="8"/>
-      <c r="F87" s="14"/>
+      <c r="F87" s="14" t="s">
+        <v>144</v>
+      </c>
       <c r="G87" s="8"/>
       <c r="H87" s="8"/>
       <c r="I87" s="8"/>
@@ -5177,10 +5209,16 @@
       <c r="AA87" s="8"/>
       <c r="AB87" s="8"/>
     </row>
-    <row r="88" spans="1:28">
-      <c r="A88" s="8"/>
-      <c r="B88" s="8"/>
-      <c r="C88" s="8"/>
+    <row r="88" spans="1:28" ht="25.5">
+      <c r="A88" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>147</v>
+      </c>
       <c r="D88" s="9"/>
       <c r="E88" s="8"/>
       <c r="F88" s="14"/>
@@ -5238,54 +5276,42 @@
       <c r="AB89" s="8"/>
     </row>
     <row r="90" spans="1:28">
-      <c r="A90" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
-      <c r="E90" s="2"/>
-      <c r="F90" s="13"/>
-      <c r="G90" s="2"/>
-      <c r="H90" s="2"/>
-      <c r="I90" s="2"/>
-      <c r="J90" s="2"/>
-      <c r="K90" s="2"/>
-      <c r="L90" s="2"/>
-      <c r="M90" s="2"/>
-      <c r="N90" s="2"/>
-      <c r="O90" s="2"/>
-      <c r="P90" s="2"/>
-      <c r="Q90" s="2"/>
-      <c r="R90" s="2"/>
-      <c r="S90" s="2"/>
-      <c r="T90" s="2"/>
-      <c r="U90" s="2"/>
-      <c r="V90" s="2"/>
-      <c r="W90" s="2"/>
-      <c r="X90" s="2"/>
-      <c r="Y90" s="2"/>
-      <c r="Z90" s="2"/>
-      <c r="AA90" s="2"/>
-      <c r="AB90" s="2"/>
-    </row>
-    <row r="91" spans="1:28" ht="25.5">
-      <c r="A91" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="B91" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="C91" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="D91" s="8"/>
+      <c r="A90" s="8"/>
+      <c r="B90" s="8"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="9"/>
+      <c r="E90" s="8"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="8"/>
+      <c r="H90" s="8"/>
+      <c r="I90" s="8"/>
+      <c r="J90" s="8"/>
+      <c r="K90" s="8"/>
+      <c r="L90" s="8"/>
+      <c r="M90" s="8"/>
+      <c r="N90" s="8"/>
+      <c r="O90" s="8"/>
+      <c r="P90" s="8"/>
+      <c r="Q90" s="8"/>
+      <c r="R90" s="8"/>
+      <c r="S90" s="8"/>
+      <c r="T90" s="8"/>
+      <c r="U90" s="8"/>
+      <c r="V90" s="8"/>
+      <c r="W90" s="8"/>
+      <c r="X90" s="8"/>
+      <c r="Y90" s="8"/>
+      <c r="Z90" s="8"/>
+      <c r="AA90" s="8"/>
+      <c r="AB90" s="8"/>
+    </row>
+    <row r="91" spans="1:28">
+      <c r="A91" s="8"/>
+      <c r="B91" s="8"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="9"/>
       <c r="E91" s="8"/>
-      <c r="F91" s="14" t="s">
-        <v>153</v>
-      </c>
+      <c r="F91" s="14"/>
       <c r="G91" s="8"/>
       <c r="H91" s="8"/>
       <c r="I91" s="8"/>
@@ -5310,57 +5336,53 @@
       <c r="AB91" s="8"/>
     </row>
     <row r="92" spans="1:28">
-      <c r="A92" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="B92" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C92" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="D92" s="8"/>
-      <c r="E92" s="8"/>
-      <c r="F92" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="G92" s="8"/>
-      <c r="H92" s="8"/>
-      <c r="I92" s="8"/>
-      <c r="J92" s="8"/>
-      <c r="K92" s="8"/>
-      <c r="L92" s="8"/>
-      <c r="M92" s="8"/>
-      <c r="N92" s="8"/>
-      <c r="O92" s="8"/>
-      <c r="P92" s="8"/>
-      <c r="Q92" s="8"/>
-      <c r="R92" s="8"/>
-      <c r="S92" s="8"/>
-      <c r="T92" s="8"/>
-      <c r="U92" s="8"/>
-      <c r="V92" s="8"/>
-      <c r="W92" s="8"/>
-      <c r="X92" s="8"/>
-      <c r="Y92" s="8"/>
-      <c r="Z92" s="8"/>
-      <c r="AA92" s="8"/>
-      <c r="AB92" s="8"/>
-    </row>
-    <row r="93" spans="1:28">
+      <c r="A92" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C92" s="2"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="13"/>
+      <c r="G92" s="2"/>
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+      <c r="J92" s="2"/>
+      <c r="K92" s="2"/>
+      <c r="L92" s="2"/>
+      <c r="M92" s="2"/>
+      <c r="N92" s="2"/>
+      <c r="O92" s="2"/>
+      <c r="P92" s="2"/>
+      <c r="Q92" s="2"/>
+      <c r="R92" s="2"/>
+      <c r="S92" s="2"/>
+      <c r="T92" s="2"/>
+      <c r="U92" s="2"/>
+      <c r="V92" s="2"/>
+      <c r="W92" s="2"/>
+      <c r="X92" s="2"/>
+      <c r="Y92" s="2"/>
+      <c r="Z92" s="2"/>
+      <c r="AA92" s="2"/>
+      <c r="AB92" s="2"/>
+    </row>
+    <row r="93" spans="1:28" ht="25.5">
       <c r="A93" s="8" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>73</v>
+        <v>152</v>
       </c>
       <c r="D93" s="8"/>
       <c r="E93" s="8"/>
       <c r="F93" s="14" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="G93" s="8"/>
       <c r="H93" s="8"/>
@@ -5387,18 +5409,18 @@
     </row>
     <row r="94" spans="1:28">
       <c r="A94" s="8" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>67</v>
+        <v>155</v>
       </c>
       <c r="D94" s="8"/>
       <c r="E94" s="8"/>
       <c r="F94" s="14" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G94" s="8"/>
       <c r="H94" s="8"/>
@@ -5424,53 +5446,57 @@
       <c r="AB94" s="8"/>
     </row>
     <row r="95" spans="1:28">
-      <c r="A95" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="B95" s="5"/>
-      <c r="C95" s="5"/>
-      <c r="D95" s="5"/>
-      <c r="E95" s="5"/>
-      <c r="F95" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="G95" s="5"/>
-      <c r="H95" s="5"/>
-      <c r="I95" s="5"/>
-      <c r="J95" s="5"/>
-      <c r="K95" s="5"/>
-      <c r="L95" s="5"/>
-      <c r="M95" s="5"/>
-      <c r="N95" s="5"/>
-      <c r="O95" s="5"/>
-      <c r="P95" s="5"/>
-      <c r="Q95" s="5"/>
-      <c r="R95" s="5"/>
-      <c r="S95" s="5"/>
-      <c r="T95" s="5"/>
-      <c r="U95" s="5"/>
-      <c r="V95" s="5"/>
-      <c r="W95" s="5"/>
-      <c r="X95" s="5"/>
-      <c r="Y95" s="5"/>
-      <c r="Z95" s="5"/>
-      <c r="AA95" s="5"/>
-      <c r="AB95" s="5"/>
+      <c r="A95" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D95" s="8"/>
+      <c r="E95" s="8"/>
+      <c r="F95" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="G95" s="8"/>
+      <c r="H95" s="8"/>
+      <c r="I95" s="8"/>
+      <c r="J95" s="8"/>
+      <c r="K95" s="8"/>
+      <c r="L95" s="8"/>
+      <c r="M95" s="8"/>
+      <c r="N95" s="8"/>
+      <c r="O95" s="8"/>
+      <c r="P95" s="8"/>
+      <c r="Q95" s="8"/>
+      <c r="R95" s="8"/>
+      <c r="S95" s="8"/>
+      <c r="T95" s="8"/>
+      <c r="U95" s="8"/>
+      <c r="V95" s="8"/>
+      <c r="W95" s="8"/>
+      <c r="X95" s="8"/>
+      <c r="Y95" s="8"/>
+      <c r="Z95" s="8"/>
+      <c r="AA95" s="8"/>
+      <c r="AB95" s="8"/>
     </row>
     <row r="96" spans="1:28">
       <c r="A96" s="8" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="D96" s="8"/>
       <c r="E96" s="8"/>
       <c r="F96" s="14" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="G96" s="8"/>
       <c r="H96" s="8"/>
@@ -5496,54 +5522,54 @@
       <c r="AB96" s="8"/>
     </row>
     <row r="97" spans="1:28">
-      <c r="A97" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="B97" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D97" s="8"/>
-      <c r="E97" s="8"/>
-      <c r="F97" s="14"/>
-      <c r="G97" s="8"/>
-      <c r="H97" s="8"/>
-      <c r="I97" s="8"/>
-      <c r="J97" s="8"/>
-      <c r="K97" s="8"/>
-      <c r="L97" s="8"/>
-      <c r="M97" s="8"/>
-      <c r="N97" s="8"/>
-      <c r="O97" s="8"/>
-      <c r="P97" s="8"/>
-      <c r="Q97" s="8"/>
-      <c r="R97" s="8"/>
-      <c r="S97" s="8"/>
-      <c r="T97" s="8"/>
-      <c r="U97" s="8"/>
-      <c r="V97" s="8"/>
-      <c r="W97" s="8"/>
-      <c r="X97" s="8"/>
-      <c r="Y97" s="8"/>
-      <c r="Z97" s="8"/>
-      <c r="AA97" s="8"/>
-      <c r="AB97" s="8"/>
+      <c r="A97" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B97" s="5"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="G97" s="5"/>
+      <c r="H97" s="5"/>
+      <c r="I97" s="5"/>
+      <c r="J97" s="5"/>
+      <c r="K97" s="5"/>
+      <c r="L97" s="5"/>
+      <c r="M97" s="5"/>
+      <c r="N97" s="5"/>
+      <c r="O97" s="5"/>
+      <c r="P97" s="5"/>
+      <c r="Q97" s="5"/>
+      <c r="R97" s="5"/>
+      <c r="S97" s="5"/>
+      <c r="T97" s="5"/>
+      <c r="U97" s="5"/>
+      <c r="V97" s="5"/>
+      <c r="W97" s="5"/>
+      <c r="X97" s="5"/>
+      <c r="Y97" s="5"/>
+      <c r="Z97" s="5"/>
+      <c r="AA97" s="5"/>
+      <c r="AB97" s="5"/>
     </row>
     <row r="98" spans="1:28">
       <c r="A98" s="8" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C98" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D98" s="8"/>
       <c r="E98" s="8"/>
-      <c r="F98" s="14"/>
+      <c r="F98" s="14" t="s">
+        <v>166</v>
+      </c>
       <c r="G98" s="8"/>
       <c r="H98" s="8"/>
       <c r="I98" s="8"/>
@@ -5569,19 +5595,17 @@
     </row>
     <row r="99" spans="1:28">
       <c r="A99" s="8" t="s">
-        <v>332</v>
+        <v>167</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>333</v>
+        <v>168</v>
       </c>
       <c r="C99" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D99" s="8"/>
       <c r="E99" s="8"/>
-      <c r="F99" s="14" t="s">
-        <v>334</v>
-      </c>
+      <c r="F99" s="14"/>
       <c r="G99" s="8"/>
       <c r="H99" s="8"/>
       <c r="I99" s="8"/>
@@ -5607,19 +5631,17 @@
     </row>
     <row r="100" spans="1:28">
       <c r="A100" s="8" t="s">
-        <v>331</v>
+        <v>169</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>347</v>
+        <v>170</v>
       </c>
       <c r="C100" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D100" s="8"/>
       <c r="E100" s="8"/>
-      <c r="F100" s="14" t="s">
-        <v>323</v>
-      </c>
+      <c r="F100" s="14"/>
       <c r="G100" s="8"/>
       <c r="H100" s="8"/>
       <c r="I100" s="8"/>
@@ -5645,18 +5667,18 @@
     </row>
     <row r="101" spans="1:28">
       <c r="A101" s="8" t="s">
-        <v>171</v>
+        <v>332</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>172</v>
+        <v>333</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D101" s="8"/>
       <c r="E101" s="8"/>
       <c r="F101" s="14" t="s">
-        <v>173</v>
+        <v>334</v>
       </c>
       <c r="G101" s="8"/>
       <c r="H101" s="8"/>
@@ -5683,17 +5705,19 @@
     </row>
     <row r="102" spans="1:28">
       <c r="A102" s="8" t="s">
-        <v>174</v>
+        <v>331</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>175</v>
+        <v>347</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D102" s="8"/>
       <c r="E102" s="8"/>
-      <c r="F102" s="14"/>
+      <c r="F102" s="14" t="s">
+        <v>323</v>
+      </c>
       <c r="G102" s="8"/>
       <c r="H102" s="8"/>
       <c r="I102" s="8"/>
@@ -5717,19 +5741,21 @@
       <c r="AA102" s="8"/>
       <c r="AB102" s="8"/>
     </row>
-    <row r="103" spans="1:28" ht="25.5">
+    <row r="103" spans="1:28">
       <c r="A103" s="8" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>178</v>
+        <v>20</v>
       </c>
       <c r="D103" s="8"/>
       <c r="E103" s="8"/>
-      <c r="F103" s="14"/>
+      <c r="F103" s="14" t="s">
+        <v>173</v>
+      </c>
       <c r="G103" s="8"/>
       <c r="H103" s="8"/>
       <c r="I103" s="8"/>
@@ -5754,46 +5780,50 @@
       <c r="AB103" s="8"/>
     </row>
     <row r="104" spans="1:28">
-      <c r="A104" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="B104" s="6"/>
-      <c r="C104" s="6"/>
-      <c r="D104" s="6"/>
-      <c r="E104" s="6"/>
-      <c r="F104" s="25"/>
-      <c r="G104" s="6"/>
-      <c r="H104" s="6"/>
-      <c r="I104" s="6"/>
-      <c r="J104" s="6"/>
-      <c r="K104" s="6"/>
-      <c r="L104" s="6"/>
-      <c r="M104" s="6"/>
-      <c r="N104" s="6"/>
-      <c r="O104" s="6"/>
-      <c r="P104" s="6"/>
-      <c r="Q104" s="6"/>
-      <c r="R104" s="6"/>
-      <c r="S104" s="6"/>
-      <c r="T104" s="6"/>
-      <c r="U104" s="6"/>
-      <c r="V104" s="6"/>
-      <c r="W104" s="6"/>
-      <c r="X104" s="6"/>
-      <c r="Y104" s="6"/>
-      <c r="Z104" s="6"/>
-      <c r="AA104" s="6"/>
-      <c r="AB104" s="6"/>
-    </row>
-    <row r="105" spans="1:28">
+      <c r="A104" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D104" s="8"/>
+      <c r="E104" s="8"/>
+      <c r="F104" s="14"/>
+      <c r="G104" s="8"/>
+      <c r="H104" s="8"/>
+      <c r="I104" s="8"/>
+      <c r="J104" s="8"/>
+      <c r="K104" s="8"/>
+      <c r="L104" s="8"/>
+      <c r="M104" s="8"/>
+      <c r="N104" s="8"/>
+      <c r="O104" s="8"/>
+      <c r="P104" s="8"/>
+      <c r="Q104" s="8"/>
+      <c r="R104" s="8"/>
+      <c r="S104" s="8"/>
+      <c r="T104" s="8"/>
+      <c r="U104" s="8"/>
+      <c r="V104" s="8"/>
+      <c r="W104" s="8"/>
+      <c r="X104" s="8"/>
+      <c r="Y104" s="8"/>
+      <c r="Z104" s="8"/>
+      <c r="AA104" s="8"/>
+      <c r="AB104" s="8"/>
+    </row>
+    <row r="105" spans="1:28" ht="25.5">
       <c r="A105" s="8" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="D105" s="8"/>
       <c r="E105" s="8"/>
@@ -5822,47 +5852,43 @@
       <c r="AB105" s="8"/>
     </row>
     <row r="106" spans="1:28">
-      <c r="A106" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="B106" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="C106" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D106" s="8"/>
-      <c r="E106" s="8"/>
-      <c r="F106" s="14"/>
-      <c r="G106" s="8"/>
-      <c r="H106" s="8"/>
-      <c r="I106" s="8"/>
-      <c r="J106" s="8"/>
-      <c r="K106" s="8"/>
-      <c r="L106" s="8"/>
-      <c r="M106" s="8"/>
-      <c r="N106" s="8"/>
-      <c r="O106" s="8"/>
-      <c r="P106" s="8"/>
-      <c r="Q106" s="8"/>
-      <c r="R106" s="8"/>
-      <c r="S106" s="8"/>
-      <c r="T106" s="8"/>
-      <c r="U106" s="8"/>
-      <c r="V106" s="8"/>
-      <c r="W106" s="8"/>
-      <c r="X106" s="8"/>
-      <c r="Y106" s="8"/>
-      <c r="Z106" s="8"/>
-      <c r="AA106" s="8"/>
-      <c r="AB106" s="8"/>
+      <c r="A106" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B106" s="6"/>
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="6"/>
+      <c r="F106" s="25"/>
+      <c r="G106" s="6"/>
+      <c r="H106" s="6"/>
+      <c r="I106" s="6"/>
+      <c r="J106" s="6"/>
+      <c r="K106" s="6"/>
+      <c r="L106" s="6"/>
+      <c r="M106" s="6"/>
+      <c r="N106" s="6"/>
+      <c r="O106" s="6"/>
+      <c r="P106" s="6"/>
+      <c r="Q106" s="6"/>
+      <c r="R106" s="6"/>
+      <c r="S106" s="6"/>
+      <c r="T106" s="6"/>
+      <c r="U106" s="6"/>
+      <c r="V106" s="6"/>
+      <c r="W106" s="6"/>
+      <c r="X106" s="6"/>
+      <c r="Y106" s="6"/>
+      <c r="Z106" s="6"/>
+      <c r="AA106" s="6"/>
+      <c r="AB106" s="6"/>
     </row>
     <row r="107" spans="1:28">
       <c r="A107" s="8" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C107" s="8" t="s">
         <v>26</v>
@@ -5895,19 +5921,17 @@
     </row>
     <row r="108" spans="1:28">
       <c r="A108" s="8" t="s">
-        <v>336</v>
+        <v>182</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>338</v>
+        <v>183</v>
       </c>
       <c r="C108" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D108" s="8"/>
       <c r="E108" s="8"/>
-      <c r="F108" s="14" t="s">
-        <v>335</v>
-      </c>
+      <c r="F108" s="14"/>
       <c r="G108" s="8"/>
       <c r="H108" s="8"/>
       <c r="I108" s="8"/>
@@ -5933,19 +5957,17 @@
     </row>
     <row r="109" spans="1:28">
       <c r="A109" s="8" t="s">
-        <v>346</v>
+        <v>184</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>345</v>
+        <v>185</v>
       </c>
       <c r="C109" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D109" s="8"/>
       <c r="E109" s="8"/>
-      <c r="F109" s="16" t="s">
-        <v>337</v>
-      </c>
+      <c r="F109" s="14"/>
       <c r="G109" s="8"/>
       <c r="H109" s="8"/>
       <c r="I109" s="8"/>
@@ -5971,17 +5993,19 @@
     </row>
     <row r="110" spans="1:28">
       <c r="A110" s="8" t="s">
-        <v>186</v>
+        <v>336</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>187</v>
+        <v>338</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D110" s="8"/>
       <c r="E110" s="8"/>
-      <c r="F110" s="14"/>
+      <c r="F110" s="14" t="s">
+        <v>335</v>
+      </c>
       <c r="G110" s="8"/>
       <c r="H110" s="8"/>
       <c r="I110" s="8"/>
@@ -6007,17 +6031,19 @@
     </row>
     <row r="111" spans="1:28">
       <c r="A111" s="8" t="s">
-        <v>188</v>
+        <v>346</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>189</v>
+        <v>345</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D111" s="8"/>
       <c r="E111" s="8"/>
-      <c r="F111" s="14"/>
+      <c r="F111" s="16" t="s">
+        <v>337</v>
+      </c>
       <c r="G111" s="8"/>
       <c r="H111" s="8"/>
       <c r="I111" s="8"/>
@@ -6043,13 +6069,13 @@
     </row>
     <row r="112" spans="1:28">
       <c r="A112" s="8" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>192</v>
+        <v>20</v>
       </c>
       <c r="D112" s="8"/>
       <c r="E112" s="8"/>
@@ -6078,46 +6104,50 @@
       <c r="AB112" s="8"/>
     </row>
     <row r="113" spans="1:28">
-      <c r="A113" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="B113" s="6"/>
-      <c r="C113" s="6"/>
-      <c r="D113" s="6"/>
-      <c r="E113" s="6"/>
-      <c r="F113" s="25"/>
-      <c r="G113" s="6"/>
-      <c r="H113" s="6"/>
-      <c r="I113" s="6"/>
-      <c r="J113" s="6"/>
-      <c r="K113" s="6"/>
-      <c r="L113" s="6"/>
-      <c r="M113" s="6"/>
-      <c r="N113" s="6"/>
-      <c r="O113" s="6"/>
-      <c r="P113" s="6"/>
-      <c r="Q113" s="6"/>
-      <c r="R113" s="6"/>
-      <c r="S113" s="6"/>
-      <c r="T113" s="6"/>
-      <c r="U113" s="6"/>
-      <c r="V113" s="6"/>
-      <c r="W113" s="6"/>
-      <c r="X113" s="6"/>
-      <c r="Y113" s="6"/>
-      <c r="Z113" s="6"/>
-      <c r="AA113" s="6"/>
-      <c r="AB113" s="6"/>
+      <c r="A113" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B113" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C113" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D113" s="8"/>
+      <c r="E113" s="8"/>
+      <c r="F113" s="14"/>
+      <c r="G113" s="8"/>
+      <c r="H113" s="8"/>
+      <c r="I113" s="8"/>
+      <c r="J113" s="8"/>
+      <c r="K113" s="8"/>
+      <c r="L113" s="8"/>
+      <c r="M113" s="8"/>
+      <c r="N113" s="8"/>
+      <c r="O113" s="8"/>
+      <c r="P113" s="8"/>
+      <c r="Q113" s="8"/>
+      <c r="R113" s="8"/>
+      <c r="S113" s="8"/>
+      <c r="T113" s="8"/>
+      <c r="U113" s="8"/>
+      <c r="V113" s="8"/>
+      <c r="W113" s="8"/>
+      <c r="X113" s="8"/>
+      <c r="Y113" s="8"/>
+      <c r="Z113" s="8"/>
+      <c r="AA113" s="8"/>
+      <c r="AB113" s="8"/>
     </row>
     <row r="114" spans="1:28">
       <c r="A114" s="8" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>26</v>
+        <v>192</v>
       </c>
       <c r="D114" s="8"/>
       <c r="E114" s="8"/>
@@ -6146,47 +6176,43 @@
       <c r="AB114" s="8"/>
     </row>
     <row r="115" spans="1:28">
-      <c r="A115" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="B115" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="C115" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D115" s="8"/>
-      <c r="E115" s="8"/>
-      <c r="F115" s="14"/>
-      <c r="G115" s="8"/>
-      <c r="H115" s="8"/>
-      <c r="I115" s="8"/>
-      <c r="J115" s="8"/>
-      <c r="K115" s="8"/>
-      <c r="L115" s="8"/>
-      <c r="M115" s="8"/>
-      <c r="N115" s="8"/>
-      <c r="O115" s="8"/>
-      <c r="P115" s="8"/>
-      <c r="Q115" s="8"/>
-      <c r="R115" s="8"/>
-      <c r="S115" s="8"/>
-      <c r="T115" s="8"/>
-      <c r="U115" s="8"/>
-      <c r="V115" s="8"/>
-      <c r="W115" s="8"/>
-      <c r="X115" s="8"/>
-      <c r="Y115" s="8"/>
-      <c r="Z115" s="8"/>
-      <c r="AA115" s="8"/>
-      <c r="AB115" s="8"/>
+      <c r="A115" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B115" s="6"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+      <c r="F115" s="25"/>
+      <c r="G115" s="6"/>
+      <c r="H115" s="6"/>
+      <c r="I115" s="6"/>
+      <c r="J115" s="6"/>
+      <c r="K115" s="6"/>
+      <c r="L115" s="6"/>
+      <c r="M115" s="6"/>
+      <c r="N115" s="6"/>
+      <c r="O115" s="6"/>
+      <c r="P115" s="6"/>
+      <c r="Q115" s="6"/>
+      <c r="R115" s="6"/>
+      <c r="S115" s="6"/>
+      <c r="T115" s="6"/>
+      <c r="U115" s="6"/>
+      <c r="V115" s="6"/>
+      <c r="W115" s="6"/>
+      <c r="X115" s="6"/>
+      <c r="Y115" s="6"/>
+      <c r="Z115" s="6"/>
+      <c r="AA115" s="6"/>
+      <c r="AB115" s="6"/>
     </row>
     <row r="116" spans="1:28">
       <c r="A116" s="8" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C116" s="8" t="s">
         <v>26</v>
@@ -6219,19 +6245,17 @@
     </row>
     <row r="117" spans="1:28">
       <c r="A117" s="8" t="s">
-        <v>339</v>
+        <v>196</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>340</v>
+        <v>197</v>
       </c>
       <c r="C117" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D117" s="8"/>
       <c r="E117" s="8"/>
-      <c r="F117" s="14" t="s">
-        <v>334</v>
-      </c>
+      <c r="F117" s="14"/>
       <c r="G117" s="8"/>
       <c r="H117" s="8"/>
       <c r="I117" s="8"/>
@@ -6257,19 +6281,17 @@
     </row>
     <row r="118" spans="1:28">
       <c r="A118" s="8" t="s">
-        <v>349</v>
+        <v>198</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>348</v>
+        <v>199</v>
       </c>
       <c r="C118" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D118" s="8"/>
       <c r="E118" s="8"/>
-      <c r="F118" s="26" t="s">
-        <v>323</v>
-      </c>
+      <c r="F118" s="14"/>
       <c r="G118" s="8"/>
       <c r="H118" s="8"/>
       <c r="I118" s="8"/>
@@ -6295,17 +6317,19 @@
     </row>
     <row r="119" spans="1:28">
       <c r="A119" s="8" t="s">
-        <v>200</v>
+        <v>339</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>201</v>
+        <v>340</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D119" s="8"/>
       <c r="E119" s="8"/>
-      <c r="F119" s="14"/>
+      <c r="F119" s="14" t="s">
+        <v>334</v>
+      </c>
       <c r="G119" s="8"/>
       <c r="H119" s="8"/>
       <c r="I119" s="8"/>
@@ -6331,17 +6355,19 @@
     </row>
     <row r="120" spans="1:28">
       <c r="A120" s="8" t="s">
-        <v>202</v>
+        <v>349</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>203</v>
+        <v>348</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D120" s="8"/>
       <c r="E120" s="8"/>
-      <c r="F120" s="14"/>
+      <c r="F120" s="26" t="s">
+        <v>323</v>
+      </c>
       <c r="G120" s="8"/>
       <c r="H120" s="8"/>
       <c r="I120" s="8"/>
@@ -6365,15 +6391,15 @@
       <c r="AA120" s="8"/>
       <c r="AB120" s="8"/>
     </row>
-    <row r="121" spans="1:28" ht="25.5">
+    <row r="121" spans="1:28">
       <c r="A121" s="8" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>178</v>
+        <v>20</v>
       </c>
       <c r="D121" s="8"/>
       <c r="E121" s="8"/>
@@ -6402,52 +6428,54 @@
       <c r="AB121" s="8"/>
     </row>
     <row r="122" spans="1:28">
-      <c r="A122" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="B122" s="6"/>
-      <c r="C122" s="6"/>
-      <c r="D122" s="6"/>
-      <c r="E122" s="6"/>
-      <c r="F122" s="25"/>
-      <c r="G122" s="6"/>
-      <c r="H122" s="6"/>
-      <c r="I122" s="6"/>
-      <c r="J122" s="6"/>
-      <c r="K122" s="6"/>
-      <c r="L122" s="6"/>
-      <c r="M122" s="6"/>
-      <c r="N122" s="6"/>
-      <c r="O122" s="6"/>
-      <c r="P122" s="6"/>
-      <c r="Q122" s="6"/>
-      <c r="R122" s="6"/>
-      <c r="S122" s="6"/>
-      <c r="T122" s="6"/>
-      <c r="U122" s="6"/>
-      <c r="V122" s="6"/>
-      <c r="W122" s="6"/>
-      <c r="X122" s="6"/>
-      <c r="Y122" s="6"/>
-      <c r="Z122" s="6"/>
-      <c r="AA122" s="6"/>
-      <c r="AB122" s="6"/>
-    </row>
-    <row r="123" spans="1:28">
+      <c r="A122" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="C122" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D122" s="8"/>
+      <c r="E122" s="8"/>
+      <c r="F122" s="14"/>
+      <c r="G122" s="8"/>
+      <c r="H122" s="8"/>
+      <c r="I122" s="8"/>
+      <c r="J122" s="8"/>
+      <c r="K122" s="8"/>
+      <c r="L122" s="8"/>
+      <c r="M122" s="8"/>
+      <c r="N122" s="8"/>
+      <c r="O122" s="8"/>
+      <c r="P122" s="8"/>
+      <c r="Q122" s="8"/>
+      <c r="R122" s="8"/>
+      <c r="S122" s="8"/>
+      <c r="T122" s="8"/>
+      <c r="U122" s="8"/>
+      <c r="V122" s="8"/>
+      <c r="W122" s="8"/>
+      <c r="X122" s="8"/>
+      <c r="Y122" s="8"/>
+      <c r="Z122" s="8"/>
+      <c r="AA122" s="8"/>
+      <c r="AB122" s="8"/>
+    </row>
+    <row r="123" spans="1:28" ht="25.5">
       <c r="A123" s="8" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>26</v>
+        <v>178</v>
       </c>
       <c r="D123" s="8"/>
       <c r="E123" s="8"/>
-      <c r="F123" s="14" t="s">
-        <v>209</v>
-      </c>
+      <c r="F123" s="14"/>
       <c r="G123" s="8"/>
       <c r="H123" s="8"/>
       <c r="I123" s="8"/>
@@ -6472,54 +6500,52 @@
       <c r="AB123" s="8"/>
     </row>
     <row r="124" spans="1:28">
-      <c r="A124" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="B124" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="C124" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D124" s="8"/>
-      <c r="E124" s="8"/>
-      <c r="F124" s="14"/>
-      <c r="G124" s="8"/>
-      <c r="H124" s="8"/>
-      <c r="I124" s="8"/>
-      <c r="J124" s="8"/>
-      <c r="K124" s="8"/>
-      <c r="L124" s="8"/>
-      <c r="M124" s="8"/>
-      <c r="N124" s="8"/>
-      <c r="O124" s="8"/>
-      <c r="P124" s="8"/>
-      <c r="Q124" s="8"/>
-      <c r="R124" s="8"/>
-      <c r="S124" s="8"/>
-      <c r="T124" s="8"/>
-      <c r="U124" s="8"/>
-      <c r="V124" s="8"/>
-      <c r="W124" s="8"/>
-      <c r="X124" s="8"/>
-      <c r="Y124" s="8"/>
-      <c r="Z124" s="8"/>
-      <c r="AA124" s="8"/>
-      <c r="AB124" s="8"/>
+      <c r="A124" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B124" s="6"/>
+      <c r="C124" s="6"/>
+      <c r="D124" s="6"/>
+      <c r="E124" s="6"/>
+      <c r="F124" s="25"/>
+      <c r="G124" s="6"/>
+      <c r="H124" s="6"/>
+      <c r="I124" s="6"/>
+      <c r="J124" s="6"/>
+      <c r="K124" s="6"/>
+      <c r="L124" s="6"/>
+      <c r="M124" s="6"/>
+      <c r="N124" s="6"/>
+      <c r="O124" s="6"/>
+      <c r="P124" s="6"/>
+      <c r="Q124" s="6"/>
+      <c r="R124" s="6"/>
+      <c r="S124" s="6"/>
+      <c r="T124" s="6"/>
+      <c r="U124" s="6"/>
+      <c r="V124" s="6"/>
+      <c r="W124" s="6"/>
+      <c r="X124" s="6"/>
+      <c r="Y124" s="6"/>
+      <c r="Z124" s="6"/>
+      <c r="AA124" s="6"/>
+      <c r="AB124" s="6"/>
     </row>
     <row r="125" spans="1:28">
       <c r="A125" s="8" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="C125" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="C125" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D125" s="8"/>
       <c r="E125" s="8"/>
-      <c r="F125" s="14"/>
+      <c r="F125" s="14" t="s">
+        <v>209</v>
+      </c>
       <c r="G125" s="8"/>
       <c r="H125" s="8"/>
       <c r="I125" s="8"/>
@@ -6545,19 +6571,17 @@
     </row>
     <row r="126" spans="1:28">
       <c r="A126" s="8" t="s">
-        <v>341</v>
+        <v>210</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>342</v>
+        <v>211</v>
       </c>
       <c r="C126" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D126" s="8"/>
       <c r="E126" s="8"/>
-      <c r="F126" s="14" t="s">
-        <v>334</v>
-      </c>
+      <c r="F126" s="14"/>
       <c r="G126" s="8"/>
       <c r="H126" s="8"/>
       <c r="I126" s="8"/>
@@ -6583,19 +6607,17 @@
     </row>
     <row r="127" spans="1:28">
       <c r="A127" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="C127" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="C127" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D127" s="8"/>
       <c r="E127" s="8"/>
-      <c r="F127" s="14" t="s">
-        <v>324</v>
-      </c>
+      <c r="F127" s="14"/>
       <c r="G127" s="8"/>
       <c r="H127" s="8"/>
       <c r="I127" s="8"/>
@@ -6621,17 +6643,19 @@
     </row>
     <row r="128" spans="1:28">
       <c r="A128" s="8" t="s">
-        <v>215</v>
+        <v>341</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>216</v>
+        <v>342</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D128" s="8"/>
       <c r="E128" s="8"/>
-      <c r="F128" s="14"/>
+      <c r="F128" s="14" t="s">
+        <v>334</v>
+      </c>
       <c r="G128" s="8"/>
       <c r="H128" s="8"/>
       <c r="I128" s="8"/>
@@ -6657,17 +6681,19 @@
     </row>
     <row r="129" spans="1:28">
       <c r="A129" s="8" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>218</v>
+        <v>350</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D129" s="8"/>
       <c r="E129" s="8"/>
-      <c r="F129" s="14"/>
+      <c r="F129" s="14" t="s">
+        <v>324</v>
+      </c>
       <c r="G129" s="8"/>
       <c r="H129" s="8"/>
       <c r="I129" s="8"/>
@@ -6693,13 +6719,13 @@
     </row>
     <row r="130" spans="1:28">
       <c r="A130" s="8" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>192</v>
+        <v>20</v>
       </c>
       <c r="D130" s="8"/>
       <c r="E130" s="8"/>
@@ -6728,9 +6754,15 @@
       <c r="AB130" s="8"/>
     </row>
     <row r="131" spans="1:28">
-      <c r="A131" s="8"/>
-      <c r="B131" s="8"/>
-      <c r="C131" s="8"/>
+      <c r="A131" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B131" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C131" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D131" s="8"/>
       <c r="E131" s="8"/>
       <c r="F131" s="14"/>
@@ -6757,51 +6789,49 @@
       <c r="AA131" s="8"/>
       <c r="AB131" s="8"/>
     </row>
-    <row r="132" spans="1:28" ht="25.5">
-      <c r="A132" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="B132" s="5"/>
-      <c r="C132" s="5"/>
-      <c r="D132" s="5"/>
-      <c r="E132" s="5"/>
-      <c r="F132" s="24" t="s">
-        <v>222</v>
-      </c>
-      <c r="G132" s="5"/>
-      <c r="H132" s="5"/>
-      <c r="I132" s="5"/>
-      <c r="J132" s="5"/>
-      <c r="K132" s="5"/>
-      <c r="L132" s="5"/>
-      <c r="M132" s="5"/>
-      <c r="N132" s="5"/>
-      <c r="O132" s="5"/>
-      <c r="P132" s="5"/>
-      <c r="Q132" s="5"/>
-      <c r="R132" s="5"/>
-      <c r="S132" s="5"/>
-      <c r="T132" s="5"/>
-      <c r="U132" s="5"/>
-      <c r="V132" s="5"/>
-      <c r="W132" s="5"/>
-      <c r="X132" s="5"/>
-      <c r="Y132" s="5"/>
-      <c r="Z132" s="5"/>
-      <c r="AA132" s="5"/>
-      <c r="AB132" s="5"/>
+    <row r="132" spans="1:28">
+      <c r="A132" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B132" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="C132" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="D132" s="8"/>
+      <c r="E132" s="8"/>
+      <c r="F132" s="14"/>
+      <c r="G132" s="8"/>
+      <c r="H132" s="8"/>
+      <c r="I132" s="8"/>
+      <c r="J132" s="8"/>
+      <c r="K132" s="8"/>
+      <c r="L132" s="8"/>
+      <c r="M132" s="8"/>
+      <c r="N132" s="8"/>
+      <c r="O132" s="8"/>
+      <c r="P132" s="8"/>
+      <c r="Q132" s="8"/>
+      <c r="R132" s="8"/>
+      <c r="S132" s="8"/>
+      <c r="T132" s="8"/>
+      <c r="U132" s="8"/>
+      <c r="V132" s="8"/>
+      <c r="W132" s="8"/>
+      <c r="X132" s="8"/>
+      <c r="Y132" s="8"/>
+      <c r="Z132" s="8"/>
+      <c r="AA132" s="8"/>
+      <c r="AB132" s="8"/>
     </row>
     <row r="133" spans="1:28">
-      <c r="A133" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="B133" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="C133" s="9"/>
+      <c r="A133" s="8"/>
+      <c r="B133" s="8"/>
+      <c r="C133" s="8"/>
       <c r="D133" s="8"/>
       <c r="E133" s="8"/>
-      <c r="F133" s="20"/>
+      <c r="F133" s="14"/>
       <c r="G133" s="8"/>
       <c r="H133" s="8"/>
       <c r="I133" s="8"/>
@@ -6825,59 +6855,51 @@
       <c r="AA133" s="8"/>
       <c r="AB133" s="8"/>
     </row>
-    <row r="134" spans="1:28">
-      <c r="A134" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="B134" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="C134" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D134" s="8"/>
-      <c r="E134" s="8"/>
-      <c r="F134" s="20" t="s">
-        <v>227</v>
-      </c>
-      <c r="G134" s="8"/>
-      <c r="H134" s="8"/>
-      <c r="I134" s="8"/>
-      <c r="J134" s="8"/>
-      <c r="K134" s="8"/>
-      <c r="L134" s="8"/>
-      <c r="M134" s="8"/>
-      <c r="N134" s="8"/>
-      <c r="O134" s="8"/>
-      <c r="P134" s="8"/>
-      <c r="Q134" s="8"/>
-      <c r="R134" s="8"/>
-      <c r="S134" s="8"/>
-      <c r="T134" s="8"/>
-      <c r="U134" s="8"/>
-      <c r="V134" s="8"/>
-      <c r="W134" s="8"/>
-      <c r="X134" s="8"/>
-      <c r="Y134" s="8"/>
-      <c r="Z134" s="8"/>
-      <c r="AA134" s="8"/>
-      <c r="AB134" s="8"/>
+    <row r="134" spans="1:28" ht="25.5">
+      <c r="A134" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="B134" s="5"/>
+      <c r="C134" s="5"/>
+      <c r="D134" s="5"/>
+      <c r="E134" s="5"/>
+      <c r="F134" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="G134" s="5"/>
+      <c r="H134" s="5"/>
+      <c r="I134" s="5"/>
+      <c r="J134" s="5"/>
+      <c r="K134" s="5"/>
+      <c r="L134" s="5"/>
+      <c r="M134" s="5"/>
+      <c r="N134" s="5"/>
+      <c r="O134" s="5"/>
+      <c r="P134" s="5"/>
+      <c r="Q134" s="5"/>
+      <c r="R134" s="5"/>
+      <c r="S134" s="5"/>
+      <c r="T134" s="5"/>
+      <c r="U134" s="5"/>
+      <c r="V134" s="5"/>
+      <c r="W134" s="5"/>
+      <c r="X134" s="5"/>
+      <c r="Y134" s="5"/>
+      <c r="Z134" s="5"/>
+      <c r="AA134" s="5"/>
+      <c r="AB134" s="5"/>
     </row>
     <row r="135" spans="1:28">
       <c r="A135" s="8" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="C135" s="9" t="s">
-        <v>26</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="C135" s="9"/>
       <c r="D135" s="8"/>
       <c r="E135" s="8"/>
-      <c r="F135" s="14" t="s">
-        <v>230</v>
-      </c>
+      <c r="F135" s="20"/>
       <c r="G135" s="8"/>
       <c r="H135" s="8"/>
       <c r="I135" s="8"/>
@@ -6903,18 +6925,18 @@
     </row>
     <row r="136" spans="1:28">
       <c r="A136" s="8" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C136" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D136" s="8"/>
       <c r="E136" s="8"/>
-      <c r="F136" s="14" t="s">
-        <v>233</v>
+      <c r="F136" s="20" t="s">
+        <v>227</v>
       </c>
       <c r="G136" s="8"/>
       <c r="H136" s="8"/>
@@ -6941,18 +6963,18 @@
     </row>
     <row r="137" spans="1:28">
       <c r="A137" s="8" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="C137" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D137" s="8"/>
       <c r="E137" s="8"/>
-      <c r="F137" s="16" t="s">
-        <v>236</v>
+      <c r="F137" s="14" t="s">
+        <v>230</v>
       </c>
       <c r="G137" s="8"/>
       <c r="H137" s="8"/>
@@ -6978,12 +7000,20 @@
       <c r="AB137" s="8"/>
     </row>
     <row r="138" spans="1:28">
-      <c r="A138" s="8"/>
-      <c r="B138" s="8"/>
-      <c r="C138" s="8"/>
-      <c r="D138" s="9"/>
+      <c r="A138" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B138" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="C138" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D138" s="8"/>
       <c r="E138" s="8"/>
-      <c r="F138" s="14"/>
+      <c r="F138" s="14" t="s">
+        <v>233</v>
+      </c>
       <c r="G138" s="8"/>
       <c r="H138" s="8"/>
       <c r="I138" s="8"/>
@@ -7008,12 +7038,20 @@
       <c r="AB138" s="8"/>
     </row>
     <row r="139" spans="1:28">
-      <c r="A139" s="8"/>
-      <c r="B139" s="8"/>
-      <c r="C139" s="8"/>
-      <c r="D139" s="9"/>
+      <c r="A139" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="B139" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="C139" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D139" s="8"/>
       <c r="E139" s="8"/>
-      <c r="F139" s="14"/>
+      <c r="F139" s="16" t="s">
+        <v>236</v>
+      </c>
       <c r="G139" s="8"/>
       <c r="H139" s="8"/>
       <c r="I139" s="8"/>
@@ -7098,54 +7136,42 @@
       <c r="AB141" s="8"/>
     </row>
     <row r="142" spans="1:28">
-      <c r="A142" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C142" s="2"/>
-      <c r="D142" s="2"/>
-      <c r="E142" s="2"/>
-      <c r="F142" s="13"/>
-      <c r="G142" s="2"/>
-      <c r="H142" s="2"/>
-      <c r="I142" s="2"/>
-      <c r="J142" s="2"/>
-      <c r="K142" s="2"/>
-      <c r="L142" s="2"/>
-      <c r="M142" s="2"/>
-      <c r="N142" s="2"/>
-      <c r="O142" s="2"/>
-      <c r="P142" s="2"/>
-      <c r="Q142" s="2"/>
-      <c r="R142" s="2"/>
-      <c r="S142" s="2"/>
-      <c r="T142" s="2"/>
-      <c r="U142" s="2"/>
-      <c r="V142" s="2"/>
-      <c r="W142" s="2"/>
-      <c r="X142" s="2"/>
-      <c r="Y142" s="2"/>
-      <c r="Z142" s="2"/>
-      <c r="AA142" s="2"/>
-      <c r="AB142" s="2"/>
-    </row>
-    <row r="143" spans="1:28" ht="25.5">
-      <c r="A143" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B143" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="C143" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="A142" s="8"/>
+      <c r="B142" s="8"/>
+      <c r="C142" s="8"/>
+      <c r="D142" s="9"/>
+      <c r="E142" s="8"/>
+      <c r="F142" s="14"/>
+      <c r="G142" s="8"/>
+      <c r="H142" s="8"/>
+      <c r="I142" s="8"/>
+      <c r="J142" s="8"/>
+      <c r="K142" s="8"/>
+      <c r="L142" s="8"/>
+      <c r="M142" s="8"/>
+      <c r="N142" s="8"/>
+      <c r="O142" s="8"/>
+      <c r="P142" s="8"/>
+      <c r="Q142" s="8"/>
+      <c r="R142" s="8"/>
+      <c r="S142" s="8"/>
+      <c r="T142" s="8"/>
+      <c r="U142" s="8"/>
+      <c r="V142" s="8"/>
+      <c r="W142" s="8"/>
+      <c r="X142" s="8"/>
+      <c r="Y142" s="8"/>
+      <c r="Z142" s="8"/>
+      <c r="AA142" s="8"/>
+      <c r="AB142" s="8"/>
+    </row>
+    <row r="143" spans="1:28">
+      <c r="A143" s="8"/>
+      <c r="B143" s="8"/>
+      <c r="C143" s="8"/>
       <c r="D143" s="9"/>
       <c r="E143" s="8"/>
-      <c r="F143" s="14" t="s">
-        <v>239</v>
-      </c>
+      <c r="F143" s="14"/>
       <c r="G143" s="8"/>
       <c r="H143" s="8"/>
       <c r="I143" s="8"/>
@@ -7170,126 +7196,122 @@
       <c r="AB143" s="8"/>
     </row>
     <row r="144" spans="1:28">
-      <c r="A144" s="10" t="s">
+      <c r="A144" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C144" s="2"/>
+      <c r="D144" s="2"/>
+      <c r="E144" s="2"/>
+      <c r="F144" s="13"/>
+      <c r="G144" s="2"/>
+      <c r="H144" s="2"/>
+      <c r="I144" s="2"/>
+      <c r="J144" s="2"/>
+      <c r="K144" s="2"/>
+      <c r="L144" s="2"/>
+      <c r="M144" s="2"/>
+      <c r="N144" s="2"/>
+      <c r="O144" s="2"/>
+      <c r="P144" s="2"/>
+      <c r="Q144" s="2"/>
+      <c r="R144" s="2"/>
+      <c r="S144" s="2"/>
+      <c r="T144" s="2"/>
+      <c r="U144" s="2"/>
+      <c r="V144" s="2"/>
+      <c r="W144" s="2"/>
+      <c r="X144" s="2"/>
+      <c r="Y144" s="2"/>
+      <c r="Z144" s="2"/>
+      <c r="AA144" s="2"/>
+      <c r="AB144" s="2"/>
+    </row>
+    <row r="145" spans="1:28" ht="25.5">
+      <c r="A145" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B145" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C145" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D145" s="9"/>
+      <c r="E145" s="8"/>
+      <c r="F145" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="G145" s="8"/>
+      <c r="H145" s="8"/>
+      <c r="I145" s="8"/>
+      <c r="J145" s="8"/>
+      <c r="K145" s="8"/>
+      <c r="L145" s="8"/>
+      <c r="M145" s="8"/>
+      <c r="N145" s="8"/>
+      <c r="O145" s="8"/>
+      <c r="P145" s="8"/>
+      <c r="Q145" s="8"/>
+      <c r="R145" s="8"/>
+      <c r="S145" s="8"/>
+      <c r="T145" s="8"/>
+      <c r="U145" s="8"/>
+      <c r="V145" s="8"/>
+      <c r="W145" s="8"/>
+      <c r="X145" s="8"/>
+      <c r="Y145" s="8"/>
+      <c r="Z145" s="8"/>
+      <c r="AA145" s="8"/>
+      <c r="AB145" s="8"/>
+    </row>
+    <row r="146" spans="1:28">
+      <c r="A146" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B144" s="10" t="s">
+      <c r="B146" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="C144" s="10" t="s">
+      <c r="C146" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D144" s="10"/>
-      <c r="E144" s="10"/>
-      <c r="F144" s="16" t="s">
+      <c r="D146" s="10"/>
+      <c r="E146" s="10"/>
+      <c r="F146" s="16" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="145" spans="1:28">
-      <c r="A145" s="10" t="s">
+    <row r="147" spans="1:28">
+      <c r="A147" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B145" s="10" t="s">
+      <c r="B147" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="C145" s="10" t="s">
+      <c r="C147" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D145" s="7"/>
-      <c r="F145" s="16" t="s">
+      <c r="D147" s="7"/>
+      <c r="F147" s="16" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="146" spans="1:28" ht="25.5">
-      <c r="A146" s="8" t="s">
+    <row r="148" spans="1:28" ht="25.5">
+      <c r="A148" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="B146" s="8" t="s">
+      <c r="B148" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="C146" s="8" t="s">
+      <c r="C148" s="8" t="s">
         <v>106</v>
-      </c>
-      <c r="D146" s="9"/>
-      <c r="E146" s="8"/>
-      <c r="F146" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="G146" s="8"/>
-      <c r="H146" s="8"/>
-      <c r="I146" s="8"/>
-      <c r="J146" s="8"/>
-      <c r="K146" s="8"/>
-      <c r="L146" s="8"/>
-      <c r="M146" s="8"/>
-      <c r="N146" s="8"/>
-      <c r="O146" s="8"/>
-      <c r="P146" s="8"/>
-      <c r="Q146" s="8"/>
-      <c r="R146" s="8"/>
-      <c r="S146" s="8"/>
-      <c r="T146" s="8"/>
-      <c r="U146" s="8"/>
-      <c r="V146" s="8"/>
-      <c r="W146" s="8"/>
-      <c r="X146" s="8"/>
-      <c r="Y146" s="8"/>
-      <c r="Z146" s="8"/>
-      <c r="AA146" s="8"/>
-      <c r="AB146" s="8"/>
-    </row>
-    <row r="147" spans="1:28">
-      <c r="A147" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="B147" s="8" t="s">
-        <v>352</v>
-      </c>
-      <c r="C147" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D147" s="9"/>
-      <c r="E147" s="8"/>
-      <c r="F147" s="14" t="s">
-        <v>351</v>
-      </c>
-      <c r="G147" s="8"/>
-      <c r="H147" s="8"/>
-      <c r="I147" s="8"/>
-      <c r="J147" s="8"/>
-      <c r="K147" s="8"/>
-      <c r="L147" s="8"/>
-      <c r="M147" s="8"/>
-      <c r="N147" s="8"/>
-      <c r="O147" s="8"/>
-      <c r="P147" s="8"/>
-      <c r="Q147" s="8"/>
-      <c r="R147" s="8"/>
-      <c r="S147" s="8"/>
-      <c r="T147" s="8"/>
-      <c r="U147" s="8"/>
-      <c r="V147" s="8"/>
-      <c r="W147" s="8"/>
-      <c r="X147" s="8"/>
-      <c r="Y147" s="8"/>
-      <c r="Z147" s="8"/>
-      <c r="AA147" s="8"/>
-      <c r="AB147" s="8"/>
-    </row>
-    <row r="148" spans="1:28">
-      <c r="A148" s="11" t="s">
-        <v>326</v>
-      </c>
-      <c r="B148" s="11" t="s">
-        <v>327</v>
-      </c>
-      <c r="C148" s="11" t="s">
-        <v>26</v>
       </c>
       <c r="D148" s="9"/>
       <c r="E148" s="8"/>
-      <c r="F148" s="19" t="s">
-        <v>328</v>
+      <c r="F148" s="14" t="s">
+        <v>246</v>
       </c>
       <c r="G148" s="8"/>
       <c r="H148" s="8"/>
@@ -7315,11 +7337,11 @@
       <c r="AB148" s="8"/>
     </row>
     <row r="149" spans="1:28">
-      <c r="A149" s="7" t="s">
-        <v>247</v>
+      <c r="A149" s="8" t="s">
+        <v>325</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>248</v>
+        <v>352</v>
       </c>
       <c r="C149" s="8" t="s">
         <v>26</v>
@@ -7327,7 +7349,7 @@
       <c r="D149" s="9"/>
       <c r="E149" s="8"/>
       <c r="F149" s="14" t="s">
-        <v>249</v>
+        <v>351</v>
       </c>
       <c r="G149" s="8"/>
       <c r="H149" s="8"/>
@@ -7353,19 +7375,19 @@
       <c r="AB149" s="8"/>
     </row>
     <row r="150" spans="1:28">
-      <c r="A150" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="B150" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C150" s="8" t="s">
+      <c r="A150" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="B150" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="C150" s="11" t="s">
         <v>26</v>
       </c>
       <c r="D150" s="9"/>
       <c r="E150" s="8"/>
-      <c r="F150" s="14" t="s">
-        <v>251</v>
+      <c r="F150" s="19" t="s">
+        <v>328</v>
       </c>
       <c r="G150" s="8"/>
       <c r="H150" s="8"/>
@@ -7391,11 +7413,11 @@
       <c r="AB150" s="8"/>
     </row>
     <row r="151" spans="1:28">
-      <c r="A151" s="8" t="s">
-        <v>252</v>
+      <c r="A151" s="7" t="s">
+        <v>247</v>
       </c>
       <c r="B151" s="8" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C151" s="8" t="s">
         <v>26</v>
@@ -7403,7 +7425,7 @@
       <c r="D151" s="9"/>
       <c r="E151" s="8"/>
       <c r="F151" s="14" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="G151" s="8"/>
       <c r="H151" s="8"/>
@@ -7430,17 +7452,19 @@
     </row>
     <row r="152" spans="1:28">
       <c r="A152" s="8" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>256</v>
+        <v>25</v>
       </c>
       <c r="C152" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D152" s="9"/>
       <c r="E152" s="8"/>
-      <c r="F152" s="14"/>
+      <c r="F152" s="14" t="s">
+        <v>251</v>
+      </c>
       <c r="G152" s="8"/>
       <c r="H152" s="8"/>
       <c r="I152" s="8"/>
@@ -7464,12 +7488,12 @@
       <c r="AA152" s="8"/>
       <c r="AB152" s="8"/>
     </row>
-    <row r="153" spans="1:28" ht="25.5">
+    <row r="153" spans="1:28">
       <c r="A153" s="8" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B153" s="8" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C153" s="8" t="s">
         <v>26</v>
@@ -7477,7 +7501,7 @@
       <c r="D153" s="9"/>
       <c r="E153" s="8"/>
       <c r="F153" s="14" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="G153" s="8"/>
       <c r="H153" s="8"/>
@@ -7504,19 +7528,17 @@
     </row>
     <row r="154" spans="1:28">
       <c r="A154" s="8" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C154" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D154" s="9"/>
       <c r="E154" s="8"/>
-      <c r="F154" s="14" t="s">
-        <v>262</v>
-      </c>
+      <c r="F154" s="14"/>
       <c r="G154" s="8"/>
       <c r="H154" s="8"/>
       <c r="I154" s="8"/>
@@ -7542,18 +7564,18 @@
     </row>
     <row r="155" spans="1:28" ht="25.5">
       <c r="A155" s="8" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C155" s="8" t="s">
-        <v>134</v>
+        <v>26</v>
       </c>
       <c r="D155" s="9"/>
       <c r="E155" s="8"/>
       <c r="F155" s="14" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="G155" s="8"/>
       <c r="H155" s="8"/>
@@ -7579,12 +7601,20 @@
       <c r="AB155" s="8"/>
     </row>
     <row r="156" spans="1:28">
-      <c r="A156" s="8"/>
-      <c r="B156" s="8"/>
-      <c r="C156" s="8"/>
+      <c r="A156" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C156" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="D156" s="9"/>
       <c r="E156" s="8"/>
-      <c r="F156" s="14"/>
+      <c r="F156" s="14" t="s">
+        <v>262</v>
+      </c>
       <c r="G156" s="8"/>
       <c r="H156" s="8"/>
       <c r="I156" s="8"/>
@@ -7608,13 +7638,21 @@
       <c r="AA156" s="8"/>
       <c r="AB156" s="8"/>
     </row>
-    <row r="157" spans="1:28">
-      <c r="A157" s="8"/>
-      <c r="B157" s="8"/>
-      <c r="C157" s="8"/>
+    <row r="157" spans="1:28" ht="25.5">
+      <c r="A157" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="B157" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="C157" s="8" t="s">
+        <v>134</v>
+      </c>
       <c r="D157" s="9"/>
       <c r="E157" s="8"/>
-      <c r="F157" s="14"/>
+      <c r="F157" s="14" t="s">
+        <v>265</v>
+      </c>
       <c r="G157" s="8"/>
       <c r="H157" s="8"/>
       <c r="I157" s="8"/>
@@ -7669,54 +7707,42 @@
       <c r="AB158" s="8"/>
     </row>
     <row r="159" spans="1:28">
-      <c r="A159" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="C159" s="2"/>
-      <c r="D159" s="2"/>
-      <c r="E159" s="2"/>
-      <c r="F159" s="13"/>
-      <c r="G159" s="2"/>
-      <c r="H159" s="2"/>
-      <c r="I159" s="2"/>
-      <c r="J159" s="2"/>
-      <c r="K159" s="2"/>
-      <c r="L159" s="2"/>
-      <c r="M159" s="2"/>
-      <c r="N159" s="2"/>
-      <c r="O159" s="2"/>
-      <c r="P159" s="2"/>
-      <c r="Q159" s="2"/>
-      <c r="R159" s="2"/>
-      <c r="S159" s="2"/>
-      <c r="T159" s="2"/>
-      <c r="U159" s="2"/>
-      <c r="V159" s="2"/>
-      <c r="W159" s="2"/>
-      <c r="X159" s="2"/>
-      <c r="Y159" s="2"/>
-      <c r="Z159" s="2"/>
-      <c r="AA159" s="2"/>
-      <c r="AB159" s="2"/>
-    </row>
-    <row r="160" spans="1:28" ht="63.75">
-      <c r="A160" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="B160" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="C160" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="D160" s="8"/>
+      <c r="A159" s="8"/>
+      <c r="B159" s="8"/>
+      <c r="C159" s="8"/>
+      <c r="D159" s="9"/>
+      <c r="E159" s="8"/>
+      <c r="F159" s="14"/>
+      <c r="G159" s="8"/>
+      <c r="H159" s="8"/>
+      <c r="I159" s="8"/>
+      <c r="J159" s="8"/>
+      <c r="K159" s="8"/>
+      <c r="L159" s="8"/>
+      <c r="M159" s="8"/>
+      <c r="N159" s="8"/>
+      <c r="O159" s="8"/>
+      <c r="P159" s="8"/>
+      <c r="Q159" s="8"/>
+      <c r="R159" s="8"/>
+      <c r="S159" s="8"/>
+      <c r="T159" s="8"/>
+      <c r="U159" s="8"/>
+      <c r="V159" s="8"/>
+      <c r="W159" s="8"/>
+      <c r="X159" s="8"/>
+      <c r="Y159" s="8"/>
+      <c r="Z159" s="8"/>
+      <c r="AA159" s="8"/>
+      <c r="AB159" s="8"/>
+    </row>
+    <row r="160" spans="1:28">
+      <c r="A160" s="8"/>
+      <c r="B160" s="8"/>
+      <c r="C160" s="8"/>
+      <c r="D160" s="9"/>
       <c r="E160" s="8"/>
-      <c r="F160" s="14" t="s">
-        <v>269</v>
-      </c>
+      <c r="F160" s="14"/>
       <c r="G160" s="8"/>
       <c r="H160" s="8"/>
       <c r="I160" s="8"/>
@@ -7740,58 +7766,54 @@
       <c r="AA160" s="8"/>
       <c r="AB160" s="8"/>
     </row>
-    <row r="161" spans="1:28" ht="51">
-      <c r="A161" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="B161" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="C161" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D161" s="8"/>
-      <c r="E161" s="8"/>
-      <c r="F161" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="G161" s="8"/>
-      <c r="H161" s="8"/>
-      <c r="I161" s="8"/>
-      <c r="J161" s="8"/>
-      <c r="K161" s="8"/>
-      <c r="L161" s="8"/>
-      <c r="M161" s="8"/>
-      <c r="N161" s="8"/>
-      <c r="O161" s="8"/>
-      <c r="P161" s="8"/>
-      <c r="Q161" s="8"/>
-      <c r="R161" s="8"/>
-      <c r="S161" s="8"/>
-      <c r="T161" s="8"/>
-      <c r="U161" s="8"/>
-      <c r="V161" s="8"/>
-      <c r="W161" s="8"/>
-      <c r="X161" s="8"/>
-      <c r="Y161" s="8"/>
-      <c r="Z161" s="8"/>
-      <c r="AA161" s="8"/>
-      <c r="AB161" s="8"/>
-    </row>
-    <row r="162" spans="1:28" ht="38.25">
+    <row r="161" spans="1:28">
+      <c r="A161" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C161" s="2"/>
+      <c r="D161" s="2"/>
+      <c r="E161" s="2"/>
+      <c r="F161" s="13"/>
+      <c r="G161" s="2"/>
+      <c r="H161" s="2"/>
+      <c r="I161" s="2"/>
+      <c r="J161" s="2"/>
+      <c r="K161" s="2"/>
+      <c r="L161" s="2"/>
+      <c r="M161" s="2"/>
+      <c r="N161" s="2"/>
+      <c r="O161" s="2"/>
+      <c r="P161" s="2"/>
+      <c r="Q161" s="2"/>
+      <c r="R161" s="2"/>
+      <c r="S161" s="2"/>
+      <c r="T161" s="2"/>
+      <c r="U161" s="2"/>
+      <c r="V161" s="2"/>
+      <c r="W161" s="2"/>
+      <c r="X161" s="2"/>
+      <c r="Y161" s="2"/>
+      <c r="Z161" s="2"/>
+      <c r="AA161" s="2"/>
+      <c r="AB161" s="2"/>
+    </row>
+    <row r="162" spans="1:28" ht="63.75">
       <c r="A162" s="8" t="s">
-        <v>273</v>
+        <v>150</v>
       </c>
       <c r="B162" s="8" t="s">
-        <v>274</v>
+        <v>151</v>
       </c>
       <c r="C162" s="8" t="s">
-        <v>134</v>
+        <v>268</v>
       </c>
       <c r="D162" s="8"/>
       <c r="E162" s="8"/>
       <c r="F162" s="14" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="G162" s="8"/>
       <c r="H162" s="8"/>
@@ -7816,20 +7838,20 @@
       <c r="AA162" s="8"/>
       <c r="AB162" s="8"/>
     </row>
-    <row r="163" spans="1:28" ht="38.25">
+    <row r="163" spans="1:28" ht="51">
       <c r="A163" s="8" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C163" s="8" t="s">
-        <v>270</v>
+        <v>134</v>
       </c>
       <c r="D163" s="8"/>
       <c r="E163" s="8"/>
       <c r="F163" s="14" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="G163" s="8"/>
       <c r="H163" s="8"/>
@@ -7854,13 +7876,21 @@
       <c r="AA163" s="8"/>
       <c r="AB163" s="8"/>
     </row>
-    <row r="164" spans="1:28">
-      <c r="A164" s="8"/>
-      <c r="B164" s="8"/>
-      <c r="C164" s="8"/>
+    <row r="164" spans="1:28" ht="38.25">
+      <c r="A164" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="B164" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C164" s="8" t="s">
+        <v>134</v>
+      </c>
       <c r="D164" s="8"/>
       <c r="E164" s="8"/>
-      <c r="F164" s="14"/>
+      <c r="F164" s="14" t="s">
+        <v>275</v>
+      </c>
       <c r="G164" s="8"/>
       <c r="H164" s="8"/>
       <c r="I164" s="8"/>
@@ -7884,13 +7914,21 @@
       <c r="AA164" s="8"/>
       <c r="AB164" s="8"/>
     </row>
-    <row r="165" spans="1:28">
-      <c r="A165" s="8"/>
-      <c r="B165" s="8"/>
-      <c r="C165" s="8"/>
+    <row r="165" spans="1:28" ht="38.25">
+      <c r="A165" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B165" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="C165" s="8" t="s">
+        <v>270</v>
+      </c>
       <c r="D165" s="8"/>
       <c r="E165" s="8"/>
-      <c r="F165" s="14"/>
+      <c r="F165" s="14" t="s">
+        <v>278</v>
+      </c>
       <c r="G165" s="8"/>
       <c r="H165" s="8"/>
       <c r="I165" s="8"/>
@@ -8005,10 +8043,64 @@
       <c r="AB168" s="8"/>
     </row>
     <row r="169" spans="1:28">
-      <c r="F169" s="23"/>
+      <c r="A169" s="8"/>
+      <c r="B169" s="8"/>
+      <c r="C169" s="8"/>
+      <c r="D169" s="8"/>
+      <c r="E169" s="8"/>
+      <c r="F169" s="14"/>
+      <c r="G169" s="8"/>
+      <c r="H169" s="8"/>
+      <c r="I169" s="8"/>
+      <c r="J169" s="8"/>
+      <c r="K169" s="8"/>
+      <c r="L169" s="8"/>
+      <c r="M169" s="8"/>
+      <c r="N169" s="8"/>
+      <c r="O169" s="8"/>
+      <c r="P169" s="8"/>
+      <c r="Q169" s="8"/>
+      <c r="R169" s="8"/>
+      <c r="S169" s="8"/>
+      <c r="T169" s="8"/>
+      <c r="U169" s="8"/>
+      <c r="V169" s="8"/>
+      <c r="W169" s="8"/>
+      <c r="X169" s="8"/>
+      <c r="Y169" s="8"/>
+      <c r="Z169" s="8"/>
+      <c r="AA169" s="8"/>
+      <c r="AB169" s="8"/>
     </row>
     <row r="170" spans="1:28">
-      <c r="F170" s="23"/>
+      <c r="A170" s="8"/>
+      <c r="B170" s="8"/>
+      <c r="C170" s="8"/>
+      <c r="D170" s="8"/>
+      <c r="E170" s="8"/>
+      <c r="F170" s="14"/>
+      <c r="G170" s="8"/>
+      <c r="H170" s="8"/>
+      <c r="I170" s="8"/>
+      <c r="J170" s="8"/>
+      <c r="K170" s="8"/>
+      <c r="L170" s="8"/>
+      <c r="M170" s="8"/>
+      <c r="N170" s="8"/>
+      <c r="O170" s="8"/>
+      <c r="P170" s="8"/>
+      <c r="Q170" s="8"/>
+      <c r="R170" s="8"/>
+      <c r="S170" s="8"/>
+      <c r="T170" s="8"/>
+      <c r="U170" s="8"/>
+      <c r="V170" s="8"/>
+      <c r="W170" s="8"/>
+      <c r="X170" s="8"/>
+      <c r="Y170" s="8"/>
+      <c r="Z170" s="8"/>
+      <c r="AA170" s="8"/>
+      <c r="AB170" s="8"/>
     </row>
     <row r="171" spans="1:28">
       <c r="F171" s="23"/>
@@ -8121,9 +8213,15 @@
     <row r="207" spans="6:6">
       <c r="F207" s="23"/>
     </row>
+    <row r="208" spans="6:6">
+      <c r="F208" s="23"/>
+    </row>
+    <row r="209" spans="6:6">
+      <c r="F209" s="23"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F49:I58"/>
+    <mergeCell ref="F51:I60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>